<commit_message>
Flag new EPSA application
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -4260,7 +4260,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -8196,7 +8196,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -8893,7 +8893,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C207" t="n">

</xml_diff>

<commit_message>
Improve Thaecia and EPSA flagging
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3476,12 +3476,12 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>Hukashaka</t>
+          <t>NPS</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -3493,11 +3493,11 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>0:04:57</t>
+          <t>0:04:56</t>
         </is>
       </c>
       <c r="G75" t="b">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=hukashaka</t>
+          <t>https://www.nationstates.net/region=nps</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -3517,28 +3517,28 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>Union of United Democratic States</t>
+          <t>Hukashaka</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0:03:25</t>
+          <t>0:03:18</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>0:05:08</t>
+          <t>0:04:57</t>
         </is>
       </c>
       <c r="G76" t="b">
@@ -3546,40 +3546,40 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
+          <t>https://www.nationstates.net/region=hukashaka</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>region with the word Tractor in it</t>
+          <t>Union of United Democratic States</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0:03:29</t>
+          <t>0:03:25</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>0:05:14</t>
+          <t>0:05:08</t>
         </is>
       </c>
       <c r="G77" t="b">
@@ -3587,40 +3587,40 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
+          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>The Kaiserreich</t>
+          <t>region with the word Tractor in it</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0:03:32</t>
+          <t>0:03:29</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>0:05:19</t>
+          <t>0:05:14</t>
         </is>
       </c>
       <c r="G78" t="b">
@@ -3628,24 +3628,24 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kaiserreich</t>
+          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Hightower</t>
+          <t>The Kaiserreich</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -3669,19 +3669,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=hightower</t>
+          <t>https://www.nationstates.net/region=the_kaiserreich</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>The Grand British Union</t>
+          <t>Hightower</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3690,19 +3690,19 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0:03:35</t>
+          <t>0:03:32</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>0:05:23</t>
+          <t>0:05:19</t>
         </is>
       </c>
       <c r="G80" t="b">
@@ -3710,40 +3710,40 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_grand_british_union</t>
+          <t>https://www.nationstates.net/region=hightower</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>Unity of the Freedom</t>
+          <t>The Grand British Union</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0:03:38</t>
+          <t>0:03:35</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>0:05:27</t>
+          <t>0:05:23</t>
         </is>
       </c>
       <c r="G81" t="b">
@@ -3751,40 +3751,40 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=unity_of_the_freedom</t>
+          <t>https://www.nationstates.net/region=the_grand_british_union</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>We should nuke the uk</t>
+          <t>Unity of the Freedom</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0:03:47</t>
+          <t>0:03:38</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>0:05:40</t>
+          <t>0:05:27</t>
         </is>
       </c>
       <c r="G82" t="b">
@@ -3792,40 +3792,40 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=we_should_nuke_the_uk</t>
+          <t>https://www.nationstates.net/region=unity_of_the_freedom</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>BoM, Ijaka, Osiris, TBH</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>The Friendly Nation</t>
+          <t>We should nuke the uk</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0:03:52</t>
+          <t>0:03:47</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>0:05:48</t>
+          <t>0:05:40</t>
         </is>
       </c>
       <c r="G83" t="b">
@@ -3833,40 +3833,40 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_friendly_nation</t>
+          <t>https://www.nationstates.net/region=we_should_nuke_the_uk</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>BoM, Ijaka, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>The west germanic provinces</t>
+          <t>The Friendly Nation</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0:04:33</t>
+          <t>0:03:52</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>410</v>
+        <v>348</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>0:06:50</t>
+          <t>0:05:48</t>
         </is>
       </c>
       <c r="G84" t="b">
@@ -3874,40 +3874,40 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
+          <t>https://www.nationstates.net/region=the_friendly_nation</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>Freedom Placas</t>
+          <t>The west germanic provinces</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>0:04:37</t>
+          <t>0:04:33</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>0:06:55</t>
+          <t>0:06:50</t>
         </is>
       </c>
       <c r="G85" t="b">
@@ -3915,24 +3915,24 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=freedom_placas</t>
+          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>Coral Reef 9</t>
+          <t>Freedom Placas</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -3944,11 +3944,11 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>0:06:56</t>
+          <t>0:06:55</t>
         </is>
       </c>
       <c r="G86" t="b">
@@ -3956,40 +3956,40 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=coral_reef_9</t>
+          <t>https://www.nationstates.net/region=freedom_placas</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>Swediztan isles</t>
+          <t>Coral Reef 9</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0:04:39</t>
+          <t>0:04:37</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>0:06:58</t>
+          <t>0:06:56</t>
         </is>
       </c>
       <c r="G87" t="b">
@@ -3997,19 +3997,19 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=swediztan_isles</t>
+          <t>https://www.nationstates.net/region=coral_reef_9</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>abstrusely</t>
+          <t>Swediztan isles</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4018,19 +4018,19 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0:04:41</t>
+          <t>0:04:39</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>0:07:02</t>
+          <t>0:06:58</t>
         </is>
       </c>
       <c r="G88" t="b">
@@ -4038,7 +4038,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=abstrusely</t>
+          <t>https://www.nationstates.net/region=swediztan_isles</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4050,7 +4050,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Freakland and Co</t>
+          <t>abstrusely</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4079,19 +4079,19 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=freakland_and_co</t>
+          <t>https://www.nationstates.net/region=abstrusely</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>The Mighty Horseland</t>
+          <t>Freakland and Co</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4100,19 +4100,19 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0:05:17</t>
+          <t>0:04:41</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>476</v>
+        <v>422</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>0:07:56</t>
+          <t>0:07:02</t>
         </is>
       </c>
       <c r="G90" t="b">
@@ -4120,19 +4120,19 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_mighty_horseland</t>
+          <t>https://www.nationstates.net/region=freakland_and_co</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>The Federation of the Hartland</t>
+          <t>The Mighty Horseland</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -4141,19 +4141,19 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>0:05:21</t>
+          <t>0:05:17</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>0:08:01</t>
+          <t>0:07:56</t>
         </is>
       </c>
       <c r="G91" t="b">
@@ -4161,40 +4161,40 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_federation_of_the_hartland</t>
+          <t>https://www.nationstates.net/region=the_mighty_horseland</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>The Panzerstanian Empire</t>
+          <t>The Federation of the Hartland</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>0:05:28</t>
+          <t>0:05:21</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>0:08:13</t>
+          <t>0:08:01</t>
         </is>
       </c>
       <c r="G92" t="b">
@@ -4202,40 +4202,40 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_panzerstanian_empire</t>
+          <t>https://www.nationstates.net/region=the_federation_of_the_hartland</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>Clown Council</t>
+          <t>The Panzerstanian Empire</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>0:05:30</t>
+          <t>0:05:28</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>0:08:16</t>
+          <t>0:08:13</t>
         </is>
       </c>
       <c r="G93" t="b">
@@ -4243,19 +4243,19 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=clown_council</t>
+          <t>https://www.nationstates.net/region=the_panzerstanian_empire</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>Osiris, TBH</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>The Great States of Fascist Nudists</t>
+          <t>Clown Council</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -4264,19 +4264,19 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>422</v>
+        <v>330</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>0:07:02</t>
+          <t>0:05:30</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>633</v>
+        <v>496</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>0:10:33</t>
+          <t>0:08:16</t>
         </is>
       </c>
       <c r="G94" t="b">
@@ -4284,24 +4284,24 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
+          <t>https://www.nationstates.net/region=clown_council</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
+          <t>Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>GAY PEOPLE</t>
+          <t>The Great States of Fascist Nudists</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -4313,11 +4313,11 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>0:10:34</t>
+          <t>0:10:33</t>
         </is>
       </c>
       <c r="G95" t="b">
@@ -4325,40 +4325,40 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=gay_people</t>
+          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>Ijaka, Osiris</t>
+          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>The Holy See of Vagen</t>
+          <t>GAY PEOPLE</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0:07:04</t>
+          <t>0:07:02</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>0:10:36</t>
+          <t>0:10:34</t>
         </is>
       </c>
       <c r="G96" t="b">
@@ -4366,24 +4366,24 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_holy_see_of_vagen</t>
+          <t>https://www.nationstates.net/region=gay_people</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Ijaka, Osiris</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>The fascist council</t>
+          <t>The Holy See of Vagen</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -4407,19 +4407,19 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_fascist_council</t>
+          <t>https://www.nationstates.net/region=the_holy_see_of_vagen</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>Wolfonia</t>
+          <t>The fascist council</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -4428,19 +4428,19 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0:07:13</t>
+          <t>0:07:04</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>0:10:49</t>
+          <t>0:10:36</t>
         </is>
       </c>
       <c r="G98" t="b">
@@ -4448,40 +4448,40 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=wolfonia</t>
+          <t>https://www.nationstates.net/region=the_fascist_council</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>EPSA, TBH</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>the democratic republic of Gaelle</t>
+          <t>Wolfonia</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0:07:18</t>
+          <t>0:07:13</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>0:10:57</t>
+          <t>0:10:49</t>
         </is>
       </c>
       <c r="G99" t="b">
@@ -4489,19 +4489,19 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_democratic_republic_of_gaelle</t>
+          <t>https://www.nationstates.net/region=wolfonia</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>Osiris, Sparkalia, TBH</t>
+          <t>EPSA, TBH</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>Fantastic</t>
+          <t>the democratic republic of Gaelle</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -4510,19 +4510,19 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0:07:21</t>
+          <t>0:07:18</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>0:11:02</t>
+          <t>0:10:57</t>
         </is>
       </c>
       <c r="G100" t="b">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=fantastic</t>
+          <t>https://www.nationstates.net/region=the_democratic_republic_of_gaelle</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -4542,28 +4542,28 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>North Arctica</t>
+          <t>Fantastic</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0:07:24</t>
+          <t>0:07:21</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>0:11:06</t>
+          <t>0:11:02</t>
         </is>
       </c>
       <c r="G101" t="b">
@@ -4571,40 +4571,40 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=north_arctica</t>
+          <t>https://www.nationstates.net/region=fantastic</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>The Islands of the Great Wrath</t>
+          <t>North Arctica</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>653</v>
+        <v>444</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>0:10:53</t>
+          <t>0:07:24</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>980</v>
+        <v>666</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>0:16:20</t>
+          <t>0:11:06</t>
         </is>
       </c>
       <c r="G102" t="b">
@@ -4612,24 +4612,24 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_islands_of_the_great_wrath</t>
+          <t>https://www.nationstates.net/region=north_arctica</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>Osiris, Sparkalia, TBH</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>absence</t>
+          <t>The Islands of the Great Wrath</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -4653,19 +4653,19 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=absence</t>
+          <t>https://www.nationstates.net/region=the_islands_of_the_great_wrath</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>BoM, Sparkalia, TBH</t>
+          <t>Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>International Socialist Assembly</t>
+          <t>absence</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -4694,40 +4694,40 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=international_socialist_assembly</t>
+          <t>https://www.nationstates.net/region=absence</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>BoM, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>FlipFault</t>
+          <t>International Socialist Assembly</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>694</v>
+        <v>653</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>0:11:34</t>
+          <t>0:10:53</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>1042</v>
+        <v>980</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>0:17:22</t>
+          <t>0:16:20</t>
         </is>
       </c>
       <c r="G105" t="b">
@@ -4735,19 +4735,19 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=flipfault</t>
+          <t>https://www.nationstates.net/region=international_socialist_assembly</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>Rebels of the Imperium</t>
+          <t>FlipFault</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4756,19 +4756,19 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>0:11:35</t>
+          <t>0:11:34</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>0:17:23</t>
+          <t>0:17:22</t>
         </is>
       </c>
       <c r="G106" t="b">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=rebels_of_the_imperium</t>
+          <t>https://www.nationstates.net/region=flipfault</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -4788,7 +4788,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>The 8th Grade Isles</t>
+          <t>Rebels of the Imperium</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -4797,19 +4797,19 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>0:11:39</t>
+          <t>0:11:35</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>1049</v>
+        <v>1043</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>0:17:29</t>
+          <t>0:17:23</t>
         </is>
       </c>
       <c r="G107" t="b">
@@ -4817,19 +4817,19 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_8th_grade_isles</t>
+          <t>https://www.nationstates.net/region=rebels_of_the_imperium</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>The Carrot Patch</t>
+          <t>The 8th Grade Isles</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4838,60 +4838,60 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>976</v>
+        <v>699</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>0:16:16</t>
+          <t>0:11:39</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>1464</v>
+        <v>1049</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>0:24:24</t>
+          <t>0:17:29</t>
         </is>
       </c>
       <c r="G108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_carrot_patch</t>
+          <t>https://www.nationstates.net/region=the_8th_grade_isles</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>Dutch Waltuh Union</t>
+          <t>Open Ocean 9</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>WFE, RO</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1004</v>
+        <v>775</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>0:16:44</t>
+          <t>0:12:55</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>1506</v>
+        <v>1163</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>0:25:06</t>
+          <t>0:19:23</t>
         </is>
       </c>
       <c r="G109" t="b">
@@ -4899,81 +4899,81 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=dutch_waltuh_union</t>
+          <t>https://www.nationstates.net/region=open_ocean_9</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>Kantrias, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>Greater Soviet Union</t>
+          <t>The Carrot Patch</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1005</v>
+        <v>976</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>0:16:45</t>
+          <t>0:16:16</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>1507</v>
+        <v>1464</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>0:25:07</t>
+          <t>0:24:24</t>
         </is>
       </c>
       <c r="G110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=greater_soviet_union</t>
+          <t>https://www.nationstates.net/region=the_carrot_patch</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>Les Gemeaux Vierge Verseau</t>
+          <t>Dutch Waltuh Union</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, RO</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>0:16:46</t>
+          <t>0:16:44</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>1509</v>
+        <v>1506</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>0:25:09</t>
+          <t>0:25:06</t>
         </is>
       </c>
       <c r="G111" t="b">
@@ -4981,40 +4981,40 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=les_gemeaux_vierge_verseau</t>
+          <t>https://www.nationstates.net/region=dutch_waltuh_union</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Kantrias, TBH</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>Barataria Bay</t>
+          <t>Greater Soviet Union</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>0:16:47</t>
+          <t>0:16:45</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>1511</v>
+        <v>1507</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>0:25:11</t>
+          <t>0:25:07</t>
         </is>
       </c>
       <c r="G112" t="b">
@@ -5022,19 +5022,19 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=barataria_bay</t>
+          <t>https://www.nationstates.net/region=greater_soviet_union</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>Sparkalia, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>The Thicc Continent</t>
+          <t>Les Gemeaux Vierge Verseau</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -5043,19 +5043,19 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>0:16:54</t>
+          <t>0:16:46</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>1521</v>
+        <v>1509</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>0:25:21</t>
+          <t>0:25:09</t>
         </is>
       </c>
       <c r="G113" t="b">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_thicc_continent</t>
+          <t>https://www.nationstates.net/region=les_gemeaux_vierge_verseau</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -5075,28 +5075,28 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>Cyberius Confederation</t>
+          <t>Barataria Bay</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>0:16:55</t>
+          <t>0:16:47</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>1522</v>
+        <v>1511</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>0:25:22</t>
+          <t>0:25:11</t>
         </is>
       </c>
       <c r="G114" t="b">
@@ -5104,40 +5104,40 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cyberius_confederation</t>
+          <t>https://www.nationstates.net/region=barataria_bay</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>BallsMoment</t>
+          <t>The Thicc Continent</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1118</v>
+        <v>1014</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>0:18:38</t>
+          <t>0:16:54</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>1677</v>
+        <v>1521</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>0:27:57</t>
+          <t>0:25:21</t>
         </is>
       </c>
       <c r="G115" t="b">
@@ -5145,40 +5145,40 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ballsmoment</t>
+          <t>https://www.nationstates.net/region=the_thicc_continent</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>BoM, Osiris</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>Kyorgia puppet storage</t>
+          <t>Cyberius Confederation</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1120</v>
+        <v>1015</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>0:18:40</t>
+          <t>0:16:55</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>1680</v>
+        <v>1522</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>0:28:00</t>
+          <t>0:25:22</t>
         </is>
       </c>
       <c r="G116" t="b">
@@ -5186,40 +5186,40 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
+          <t>https://www.nationstates.net/region=cyberius_confederation</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>EPSA, Lily, Osiris, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>SALMEGIA</t>
+          <t>Coffee House</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1121</v>
+        <v>1091</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>0:18:41</t>
+          <t>0:18:11</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>1682</v>
+        <v>1636</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>0:28:02</t>
+          <t>0:27:16</t>
         </is>
       </c>
       <c r="G117" t="b">
@@ -5227,40 +5227,40 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=salmegia</t>
+          <t>https://www.nationstates.net/region=coffee_house</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>The Empire Of The Magisterium</t>
+          <t>BallsMoment</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>0:18:43</t>
+          <t>0:18:38</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>1684</v>
+        <v>1677</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>0:28:04</t>
+          <t>0:27:57</t>
         </is>
       </c>
       <c r="G118" t="b">
@@ -5268,40 +5268,40 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_empire_of_the_magisterium</t>
+          <t>https://www.nationstates.net/region=ballsmoment</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>BoM, Osiris</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>Agia Germania Anest</t>
+          <t>Kyorgia puppet storage</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>0:18:43</t>
+          <t>0:18:40</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>0:28:05</t>
+          <t>0:28:00</t>
         </is>
       </c>
       <c r="G119" t="b">
@@ -5309,40 +5309,40 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=agia_germania_anest</t>
+          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>EPSA, Lily, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>accompaniment</t>
+          <t>SALMEGIA</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>0:18:44</t>
+          <t>0:18:41</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>1686</v>
+        <v>1682</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>0:28:06</t>
+          <t>0:28:02</t>
         </is>
       </c>
       <c r="G120" t="b">
@@ -5350,40 +5350,40 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=accompaniment</t>
+          <t>https://www.nationstates.net/region=salmegia</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>Roar</t>
+          <t>The Empire Of The Magisterium</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>0:18:45</t>
+          <t>0:18:43</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>0:28:07</t>
+          <t>0:28:04</t>
         </is>
       </c>
       <c r="G121" t="b">
@@ -5391,40 +5391,40 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=roar</t>
+          <t>https://www.nationstates.net/region=the_empire_of_the_magisterium</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>Volantis</t>
+          <t>Agia Germania Anest</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>0:18:45</t>
+          <t>0:18:43</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>0:28:08</t>
+          <t>0:28:05</t>
         </is>
       </c>
       <c r="G122" t="b">
@@ -5432,40 +5432,40 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=volantis</t>
+          <t>https://www.nationstates.net/region=agia_germania_anest</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>Sus amoungus</t>
+          <t>accompaniment</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>0:18:46</t>
+          <t>0:18:44</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>0:28:09</t>
+          <t>0:28:06</t>
         </is>
       </c>
       <c r="G123" t="b">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=sus_amoungus</t>
+          <t>https://www.nationstates.net/region=accompaniment</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -5485,28 +5485,28 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>Cosmopolitan Convention</t>
+          <t>Roar</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0:18:48</t>
+          <t>0:18:45</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>1692</v>
+        <v>1687</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>0:28:12</t>
+          <t>0:28:07</t>
         </is>
       </c>
       <c r="G124" t="b">
@@ -5514,40 +5514,40 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cosmopolitan_convention</t>
+          <t>https://www.nationstates.net/region=roar</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Blood</t>
+          <t>Volantis</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>0:18:49</t>
+          <t>0:18:45</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>1694</v>
+        <v>1688</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>0:28:14</t>
+          <t>0:28:08</t>
         </is>
       </c>
       <c r="G125" t="b">
@@ -5555,19 +5555,19 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
+          <t>https://www.nationstates.net/region=volantis</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily, TBH</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>NVIDIA GeForce</t>
+          <t>Sus amoungus</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -5576,19 +5576,19 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>0:18:50</t>
+          <t>0:18:46</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>1695</v>
+        <v>1689</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>0:28:15</t>
+          <t>0:28:09</t>
         </is>
       </c>
       <c r="G126" t="b">
@@ -5596,19 +5596,19 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=nvidia_geforce</t>
+          <t>https://www.nationstates.net/region=sus_amoungus</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>Sraqn Genc</t>
+          <t>Cosmopolitan Convention</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -5617,19 +5617,19 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>0:18:52</t>
+          <t>0:18:48</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>1699</v>
+        <v>1692</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>0:28:19</t>
+          <t>0:28:12</t>
         </is>
       </c>
       <c r="G127" t="b">
@@ -5637,40 +5637,40 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=sraqn_genc</t>
+          <t>https://www.nationstates.net/region=cosmopolitan_convention</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>Stellar Crystal Tavern</t>
+          <t>The Brotherhood of Blood</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1226</v>
+        <v>1129</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>0:20:26</t>
+          <t>0:18:49</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>1839</v>
+        <v>1694</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>0:30:39</t>
+          <t>0:28:14</t>
         </is>
       </c>
       <c r="G128" t="b">
@@ -5678,40 +5678,40 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>Osiris, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Land of Places</t>
+          <t>NVIDIA GeForce</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1257</v>
+        <v>1130</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>0:20:57</t>
+          <t>0:18:50</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>1886</v>
+        <v>1695</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>0:31:26</t>
+          <t>0:28:15</t>
         </is>
       </c>
       <c r="G129" t="b">
@@ -5719,40 +5719,40 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=land_of_places</t>
+          <t>https://www.nationstates.net/region=nvidia_geforce</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>Union of Green Socialist Nations</t>
+          <t>Sraqn Genc</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1609</v>
+        <v>1132</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>0:26:49</t>
+          <t>0:18:52</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>2413</v>
+        <v>1699</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>0:40:13</t>
+          <t>0:28:19</t>
         </is>
       </c>
       <c r="G130" t="b">
@@ -5760,40 +5760,40 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_green_socialist_nations</t>
+          <t>https://www.nationstates.net/region=sraqn_genc</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>StArry Nuggets</t>
+          <t>Stellar Crystal Tavern</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1742</v>
+        <v>1226</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>0:29:02</t>
+          <t>0:20:26</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>2613</v>
+        <v>1839</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>0:43:33</t>
+          <t>0:30:39</t>
         </is>
       </c>
       <c r="G131" t="b">
@@ -5801,19 +5801,19 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=starry_nuggets</t>
+          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>The Kibble Kingdom</t>
+          <t>Land of Places</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -5822,19 +5822,19 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1763</v>
+        <v>1257</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>0:29:23</t>
+          <t>0:20:57</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>2644</v>
+        <v>1886</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>0:44:04</t>
+          <t>0:31:26</t>
         </is>
       </c>
       <c r="G132" t="b">
@@ -5842,7 +5842,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kibble_kingdom</t>
+          <t>https://www.nationstates.net/region=land_of_places</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -5854,28 +5854,28 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>The Estamindian Island Chain</t>
+          <t>Nowhere</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1868</v>
+        <v>1341</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>0:31:08</t>
+          <t>0:22:21</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>2803</v>
+        <v>2012</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>0:46:43</t>
+          <t>0:33:32</t>
         </is>
       </c>
       <c r="G133" t="b">
@@ -5883,40 +5883,40 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_estamindian_island_chain</t>
+          <t>https://www.nationstates.net/region=nowhere</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>Regional Officers</t>
+          <t>Union of Green Socialist Nations</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1878</v>
+        <v>1609</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>0:31:18</t>
+          <t>0:26:49</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>2817</v>
+        <v>2413</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>0:46:57</t>
+          <t>0:40:13</t>
         </is>
       </c>
       <c r="G134" t="b">
@@ -5924,19 +5924,19 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=regional_officers</t>
+          <t>https://www.nationstates.net/region=union_of_green_socialist_nations</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>Richardsonson</t>
+          <t>StArry Nuggets</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -5945,19 +5945,19 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1903</v>
+        <v>1742</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>0:31:43</t>
+          <t>0:29:02</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>2855</v>
+        <v>2613</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>0:47:35</t>
+          <t>0:43:33</t>
         </is>
       </c>
       <c r="G135" t="b">
@@ -5965,7 +5965,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=richardsonson</t>
+          <t>https://www.nationstates.net/region=starry_nuggets</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -5977,7 +5977,7 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Malice Girl Scouts</t>
+          <t>The Kibble Kingdom</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -5986,19 +5986,19 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2249</v>
+        <v>1763</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>0:37:29</t>
+          <t>0:29:23</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>3373</v>
+        <v>2644</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>0:56:13</t>
+          <t>0:44:04</t>
         </is>
       </c>
       <c r="G136" t="b">
@@ -6006,19 +6006,19 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
+          <t>https://www.nationstates.net/region=the_kibble_kingdom</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>Cretanja Queendom</t>
+          <t>The Estamindian Island Chain</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -6027,19 +6027,19 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2291</v>
+        <v>1868</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>0:38:11</t>
+          <t>0:31:08</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>3437</v>
+        <v>2803</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>0:57:17</t>
+          <t>0:46:43</t>
         </is>
       </c>
       <c r="G137" t="b">
@@ -6047,40 +6047,40 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cretanja_queendom</t>
+          <t>https://www.nationstates.net/region=the_estamindian_island_chain</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>The Collective</t>
+          <t>Regional Officers</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>2296</v>
+        <v>1878</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>0:38:16</t>
+          <t>0:31:18</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>3444</v>
+        <v>2817</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>0:57:24</t>
+          <t>0:46:57</t>
         </is>
       </c>
       <c r="G138" t="b">
@@ -6088,40 +6088,40 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_collective</t>
+          <t>https://www.nationstates.net/region=regional_officers</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>Malphe</t>
+          <t>Richardsonson</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2680</v>
+        <v>1903</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>0:44:40</t>
+          <t>0:31:43</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>4020</v>
+        <v>2855</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>1:07:00</t>
+          <t>0:47:35</t>
         </is>
       </c>
       <c r="G139" t="b">
@@ -6129,19 +6129,19 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=malphe</t>
+          <t>https://www.nationstates.net/region=richardsonson</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>Lily, Osiris</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>Violet Irises</t>
+          <t>The Brotherhood of Malice Girl Scouts</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -6150,19 +6150,19 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2695</v>
+        <v>2249</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>0:44:55</t>
+          <t>0:37:29</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>4042</v>
+        <v>3373</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>1:07:22</t>
+          <t>0:56:13</t>
         </is>
       </c>
       <c r="G140" t="b">
@@ -6170,40 +6170,40 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=violet_irises</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>Submissive and Raidable</t>
+          <t>raiding am I right</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>2895</v>
+        <v>2278</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>0:48:15</t>
+          <t>0:37:58</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>4342</v>
+        <v>3417</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>1:12:22</t>
+          <t>0:56:57</t>
         </is>
       </c>
       <c r="G141" t="b">
@@ -6211,40 +6211,40 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+          <t>https://www.nationstates.net/region=raiding_am_i_right</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>Eastern American Union</t>
+          <t>Cretanja Queendom</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2941</v>
+        <v>2291</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>0:49:01</t>
+          <t>0:38:11</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>4411</v>
+        <v>3437</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>1:13:31</t>
+          <t>0:57:17</t>
         </is>
       </c>
       <c r="G142" t="b">
@@ -6252,92 +6252,338 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=eastern_american_union</t>
+          <t>https://www.nationstates.net/region=cretanja_queendom</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>The Collective</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>3189</v>
+        <v>2296</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>0:53:09</t>
+          <t>0:38:16</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>4784</v>
+        <v>3444</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>1:19:44</t>
+          <t>0:57:24</t>
         </is>
       </c>
       <c r="G143" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ben</t>
+          <t>https://www.nationstates.net/region=the_collective</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
+          <t>Malphe</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2680</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>0:44:40</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>4020</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>1:07:00</t>
+        </is>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=malphe</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>Lily, Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>Violet Irises</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>2695</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>0:44:55</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>4042</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>1:07:22</t>
+        </is>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=violet_irises</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>TBH</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>Submissive and Raidable</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>2895</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>0:48:15</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>4342</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>1:12:22</t>
+        </is>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>BoM</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>Eastern American Union</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>2941</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>0:49:01</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>4411</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>1:13:31</t>
+        </is>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=eastern_american_union</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Lily, TBH</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>3189</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0:53:09</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>4784</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>1:19:44</t>
+        </is>
+      </c>
+      <c r="G148" t="b">
+        <v>1</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=ben</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>The Fifth Sovereign Charter</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>WFE, RO</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>3196</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0:53:16</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>4794</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>1:19:54</t>
+        </is>
+      </c>
+      <c r="G149" t="b">
+        <v>0</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=the_fifth_sovereign_charter</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
+        <is>
           <t>Brest Oblast</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
+      <c r="B150" t="inlineStr">
         <is>
           <t>Embassies</t>
         </is>
       </c>
-      <c r="C144" t="n">
+      <c r="C150" t="n">
         <v>3437</v>
       </c>
-      <c r="D144" t="inlineStr">
+      <c r="D150" t="inlineStr">
         <is>
           <t>0:57:17</t>
         </is>
       </c>
-      <c r="E144" t="n">
+      <c r="E150" t="n">
         <v>5156</v>
       </c>
-      <c r="F144" t="inlineStr">
+      <c r="F150" t="inlineStr">
         <is>
           <t>1:25:56</t>
         </is>
       </c>
-      <c r="G144" t="b">
-        <v>0</v>
-      </c>
-      <c r="H144" t="inlineStr">
+      <c r="G150" t="b">
+        <v>0</v>
+      </c>
+      <c r="H150" t="inlineStr">
         <is>
           <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
-      <c r="I144" t="inlineStr">
+      <c r="I150" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Add practice region flagging
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="29 March 2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="30 March 2023" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,19 +492,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0:01:03</t>
+          <t>0:01:09</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:01:34</t>
+          <t>0:01:44</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -529,23 +529,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0:01:04</t>
+          <t>0:01:11</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0:01:36</t>
+          <t>0:01:46</t>
         </is>
       </c>
       <c r="G3" t="b">
@@ -574,19 +574,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0:01:09</t>
+          <t>0:01:15</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:01:44</t>
+          <t>0:01:52</t>
         </is>
       </c>
       <c r="G4" t="b">
@@ -615,19 +615,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0:01:10</t>
+          <t>0:01:15</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:01:45</t>
+          <t>0:01:53</t>
         </is>
       </c>
       <c r="G5" t="b">
@@ -656,19 +656,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0:01:11</t>
+          <t>0:01:15</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:01:46</t>
+          <t>0:01:53</t>
         </is>
       </c>
       <c r="G6" t="b">
@@ -688,28 +688,28 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Imperial County</t>
+          <t>Card2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0:01:17</t>
+          <t>0:01:24</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:01:55</t>
+          <t>0:02:06</t>
         </is>
       </c>
       <c r="G7" t="b">
@@ -717,7 +717,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=imperial_county</t>
+          <t>https://www.nationstates.net/region=card2025</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -729,7 +729,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Card2025</t>
+          <t>Matamo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -738,19 +738,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0:01:27</t>
+          <t>0:01:34</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:02:10</t>
+          <t>0:02:22</t>
         </is>
       </c>
       <c r="G8" t="b">
@@ -758,7 +758,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=card2025</t>
+          <t>https://www.nationstates.net/region=matamo</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -770,7 +770,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Matamo</t>
+          <t>Renem</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -779,19 +779,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0:01:41</t>
+          <t>0:01:38</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:02:32</t>
+          <t>0:02:28</t>
         </is>
       </c>
       <c r="G9" t="b">
@@ -799,7 +799,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=matamo</t>
+          <t>https://www.nationstates.net/region=renem</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -811,28 +811,28 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Renem</t>
+          <t>Crusaders of Guadalupe</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0:01:45</t>
+          <t>0:01:40</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:02:38</t>
+          <t>0:02:30</t>
         </is>
       </c>
       <c r="G10" t="b">
@@ -840,19 +840,19 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=renem</t>
+          <t>https://www.nationstates.net/region=crusaders_of_guadalupe</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Ijaka, Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Crusaders of Guadalupe</t>
+          <t>Uman Raion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -861,19 +861,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0:01:47</t>
+          <t>0:01:40</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:02:41</t>
+          <t>0:02:30</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -881,40 +881,40 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=crusaders_of_guadalupe</t>
+          <t>https://www.nationstates.net/region=uman_raion</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Uman Raion</t>
+          <t>kill antifa</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>WFE, RO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0:01:48</t>
+          <t>0:01:40</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:02:42</t>
+          <t>0:02:30</t>
         </is>
       </c>
       <c r="G12" t="b">
@@ -922,40 +922,40 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=uman_raion</t>
+          <t>https://www.nationstates.net/region=kill_antifa</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Kantrias, TBH</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>kill antifa</t>
+          <t>Eroias</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WFE, RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0:01:48</t>
+          <t>0:01:40</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:02:42</t>
+          <t>0:02:30</t>
         </is>
       </c>
       <c r="G13" t="b">
@@ -963,40 +963,40 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kill_antifa</t>
+          <t>https://www.nationstates.net/region=eroias</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Kantrias, TBH</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Eroias</t>
+          <t>The Democratic Group Of Asia</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0:01:48</t>
+          <t>0:01:42</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:02:42</t>
+          <t>0:02:33</t>
         </is>
       </c>
       <c r="G14" t="b">
@@ -1004,40 +1004,40 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=eroias</t>
+          <t>https://www.nationstates.net/region=the_democratic_group_of_asia</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>The Democratic Group Of Asia</t>
+          <t>Dragonborn Confederate</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0:01:50</t>
+          <t>0:01:42</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:02:45</t>
+          <t>0:02:34</t>
         </is>
       </c>
       <c r="G15" t="b">
@@ -1045,40 +1045,40 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_democratic_group_of_asia</t>
+          <t>https://www.nationstates.net/region=dragonborn_confederate</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Dragonborn Confederate</t>
+          <t>The Confederacy of German States</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0:01:51</t>
+          <t>0:01:42</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:02:46</t>
+          <t>0:02:34</t>
         </is>
       </c>
       <c r="G16" t="b">
@@ -1086,40 +1086,40 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=dragonborn_confederate</t>
+          <t>https://www.nationstates.net/region=the_confederacy_of_german_states</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>The Confederacy of German States</t>
+          <t>Solar Union</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0:01:51</t>
+          <t>0:01:43</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:02:46</t>
+          <t>0:02:35</t>
         </is>
       </c>
       <c r="G17" t="b">
@@ -1127,40 +1127,40 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_confederacy_of_german_states</t>
+          <t>https://www.nationstates.net/region=solar_union</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Solar Union</t>
+          <t>Yusmoydal</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0:01:51</t>
+          <t>0:01:57</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0:02:47</t>
+          <t>0:02:55</t>
         </is>
       </c>
       <c r="G18" t="b">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=solar_union</t>
+          <t>https://www.nationstates.net/region=yusmoydal</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Yusmoydal</t>
+          <t>The gamma quadrant</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1189,19 +1189,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0:02:13</t>
+          <t>0:01:57</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0:03:20</t>
+          <t>0:02:56</t>
         </is>
       </c>
       <c r="G19" t="b">
@@ -1209,19 +1209,19 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=yusmoydal</t>
+          <t>https://www.nationstates.net/region=the_gamma_quadrant</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Ascensionsen</t>
+          <t>Pride Rock</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1230,19 +1230,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0:02:13</t>
+          <t>0:02:05</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0:03:20</t>
+          <t>0:03:07</t>
         </is>
       </c>
       <c r="G20" t="b">
@@ -1250,19 +1250,19 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ascensionsen</t>
+          <t>https://www.nationstates.net/region=pride_rock</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>ERN</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>The gamma quadrant</t>
+          <t>The United World Region</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1271,19 +1271,19 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0:02:14</t>
+          <t>0:02:05</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0:03:21</t>
+          <t>0:03:08</t>
         </is>
       </c>
       <c r="G21" t="b">
@@ -1291,40 +1291,40 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_gamma_quadrant</t>
+          <t>https://www.nationstates.net/region=the_united_world_region</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Owls</t>
+          <t>Northern Ameria</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0:02:14</t>
+          <t>0:02:09</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0:03:21</t>
+          <t>0:03:14</t>
         </is>
       </c>
       <c r="G22" t="b">
@@ -1332,24 +1332,24 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=owls</t>
+          <t>https://www.nationstates.net/region=northern_ameria</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Sovishire farmboys</t>
+          <t>The UN Of The Universal Republic</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1373,40 +1373,40 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=sovishire_farmboys</t>
+          <t>https://www.nationstates.net/region=the_un_of_the_universal_republic</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Pride Rock</t>
+          <t>accession</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0:02:18</t>
+          <t>0:02:15</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0:03:26</t>
+          <t>0:03:22</t>
         </is>
       </c>
       <c r="G24" t="b">
@@ -1414,40 +1414,40 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=pride_rock</t>
+          <t>https://www.nationstates.net/region=accession</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>ERN</t>
+          <t>BoM, Osiris</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>The United World Region</t>
+          <t>The Jewel Robotox Nations</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0:02:18</t>
+          <t>0:02:17</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0:03:27</t>
+          <t>0:03:25</t>
         </is>
       </c>
       <c r="G25" t="b">
@@ -1455,40 +1455,40 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_united_world_region</t>
+          <t>https://www.nationstates.net/region=the_jewel_robotox_nations</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Northern Ameria</t>
+          <t>Goth Girls United</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0:02:26</t>
+          <t>0:02:19</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0:03:39</t>
+          <t>0:03:29</t>
         </is>
       </c>
       <c r="G26" t="b">
@@ -1496,40 +1496,40 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=northern_ameria</t>
+          <t>https://www.nationstates.net/region=goth_girls_united</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Atlae</t>
+          <t>Budget Crackheads</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0:02:27</t>
+          <t>0:02:25</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0:03:40</t>
+          <t>0:03:37</t>
         </is>
       </c>
       <c r="G27" t="b">
@@ -1537,40 +1537,40 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=atlae</t>
+          <t>https://www.nationstates.net/region=budget_crackheads</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>The UN Of The Universal Republic</t>
+          <t>Union of Dystopias</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0:02:33</t>
+          <t>0:02:28</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0:03:50</t>
+          <t>0:03:42</t>
         </is>
       </c>
       <c r="G28" t="b">
@@ -1578,40 +1578,40 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_un_of_the_universal_republic</t>
+          <t>https://www.nationstates.net/region=union_of_dystopias</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ijaka, Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>accession</t>
+          <t>The Koprulu Sector</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0:02:33</t>
+          <t>0:02:38</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0:03:50</t>
+          <t>0:03:57</t>
         </is>
       </c>
       <c r="G29" t="b">
@@ -1619,40 +1619,40 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=accession</t>
+          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>BoM, Osiris</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>The Jewel Robotox Nations</t>
+          <t>South Asian Association for Cooperation</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0:02:36</t>
+          <t>0:02:39</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0:03:54</t>
+          <t>0:03:59</t>
         </is>
       </c>
       <c r="G30" t="b">
@@ -1660,40 +1660,40 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_jewel_robotox_nations</t>
+          <t>https://www.nationstates.net/region=south_asian_association_for_cooperation</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Goth Girls United</t>
+          <t>accented</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0:02:39</t>
+          <t>0:02:46</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0:03:59</t>
+          <t>0:04:10</t>
         </is>
       </c>
       <c r="G31" t="b">
@@ -1701,40 +1701,40 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=goth_girls_united</t>
+          <t>https://www.nationstates.net/region=accented</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Sparkalia, TBH</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Budget Crackheads</t>
+          <t>Perkoempoelan Koecing Koecing</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0:02:44</t>
+          <t>0:03:13</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>246</v>
+        <v>290</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0:04:06</t>
+          <t>0:04:50</t>
         </is>
       </c>
       <c r="G32" t="b">
@@ -1742,19 +1742,19 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=budget_crackheads</t>
+          <t>https://www.nationstates.net/region=perkoempoelan_koecing_koecing</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Union of Dystopias</t>
+          <t>United Fascist Territory of Waschuster</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1763,19 +1763,19 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0:02:47</t>
+          <t>0:03:15</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0:04:11</t>
+          <t>0:04:53</t>
         </is>
       </c>
       <c r="G33" t="b">
@@ -1783,19 +1783,19 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_dystopias</t>
+          <t>https://www.nationstates.net/region=united_fascist_territory_of_waschuster</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Ukrayina</t>
+          <t>Unified Capitalist Alliance</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1804,19 +1804,19 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0:02:48</t>
+          <t>0:03:15</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>252</v>
+        <v>293</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0:04:12</t>
+          <t>0:04:53</t>
         </is>
       </c>
       <c r="G34" t="b">
@@ -1824,40 +1824,40 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ukrayina</t>
+          <t>https://www.nationstates.net/region=unified_capitalist_alliance</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>The Koprulu Sector</t>
+          <t>Archination</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0:03:05</t>
+          <t>0:03:16</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0:04:37</t>
+          <t>0:04:54</t>
         </is>
       </c>
       <c r="G35" t="b">
@@ -1865,40 +1865,40 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
+          <t>https://www.nationstates.net/region=archination</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>South Asian Association for Cooperation</t>
+          <t>NPS</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0:03:06</t>
+          <t>0:03:21</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0:04:39</t>
+          <t>0:05:01</t>
         </is>
       </c>
       <c r="G36" t="b">
@@ -1906,19 +1906,19 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=south_asian_association_for_cooperation</t>
+          <t>https://www.nationstates.net/region=nps</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>accented</t>
+          <t>Hukashaka</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1927,19 +1927,19 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0:03:11</t>
+          <t>0:03:21</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0:04:47</t>
+          <t>0:05:02</t>
         </is>
       </c>
       <c r="G37" t="b">
@@ -1947,40 +1947,40 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=accented</t>
+          <t>https://www.nationstates.net/region=hukashaka</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>The Kaisers</t>
+          <t>New Nortvia</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0:03:14</t>
+          <t>0:03:24</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0:04:51</t>
+          <t>0:05:05</t>
         </is>
       </c>
       <c r="G38" t="b">
@@ -1988,19 +1988,19 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kaisers</t>
+          <t>https://www.nationstates.net/region=new_nortvia</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Polcom</t>
+          <t>Union of United Democratic States</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2009,19 +2009,19 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0:03:44</t>
+          <t>0:03:24</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>336</v>
+        <v>305</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0:05:36</t>
+          <t>0:05:05</t>
         </is>
       </c>
       <c r="G39" t="b">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=polcom</t>
+          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2041,12 +2041,12 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Perkoempoelan Koecing Koecing</t>
+          <t>region with the word Tractor in it</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -2066,28 +2066,28 @@
         </is>
       </c>
       <c r="G40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=perkoempoelan_koecing_koecing</t>
+          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Sparkalia, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>United Fascist Territory of Waschuster</t>
+          <t>The Kaiserreich</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -2099,11 +2099,11 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0:05:42</t>
+          <t>0:05:43</t>
         </is>
       </c>
       <c r="G41" t="b">
@@ -2111,40 +2111,40 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=united_fascist_territory_of_waschuster</t>
+          <t>https://www.nationstates.net/region=the_kaiserreich</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Unified Capitalist Alliance</t>
+          <t>The west germanic provinces</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>228</v>
+        <v>295</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0:03:48</t>
+          <t>0:04:55</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>343</v>
+        <v>443</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0:05:43</t>
+          <t>0:07:23</t>
         </is>
       </c>
       <c r="G42" t="b">
@@ -2152,40 +2152,40 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=unified_capitalist_alliance</t>
+          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Archination</t>
+          <t>Subaquatic</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>228</v>
+        <v>297</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0:03:48</t>
+          <t>0:04:57</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>343</v>
+        <v>446</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0:05:43</t>
+          <t>0:07:26</t>
         </is>
       </c>
       <c r="G43" t="b">
@@ -2193,40 +2193,40 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=archination</t>
+          <t>https://www.nationstates.net/region=subaquatic</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>NPS</t>
+          <t>abstrusely</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>230</v>
+        <v>305</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0:03:50</t>
+          <t>0:05:05</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>345</v>
+        <v>458</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0:05:45</t>
+          <t>0:07:38</t>
         </is>
       </c>
       <c r="G44" t="b">
@@ -2234,19 +2234,19 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=nps</t>
+          <t>https://www.nationstates.net/region=abstrusely</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Hukashaka</t>
+          <t>Freakland and Co</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2255,19 +2255,19 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0:03:51</t>
+          <t>0:05:05</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>346</v>
+        <v>458</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0:05:46</t>
+          <t>0:07:38</t>
         </is>
       </c>
       <c r="G45" t="b">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=hukashaka</t>
+          <t>https://www.nationstates.net/region=freakland_and_co</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2287,7 +2287,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>New Nortvia</t>
+          <t>Commonwealth of Diverse Nations</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2296,19 +2296,19 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>234</v>
+        <v>330</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0:03:54</t>
+          <t>0:05:30</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>351</v>
+        <v>495</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0:05:51</t>
+          <t>0:08:15</t>
         </is>
       </c>
       <c r="G46" t="b">
@@ -2316,40 +2316,40 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=new_nortvia</t>
+          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Osiris, Sparkalia, TBH</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Union of United Democratic States</t>
+          <t>The Great States of Fascist Nudists</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>234</v>
+        <v>443</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0:03:54</t>
+          <t>0:07:23</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>351</v>
+        <v>665</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0:05:51</t>
+          <t>0:11:05</t>
         </is>
       </c>
       <c r="G47" t="b">
@@ -2357,19 +2357,19 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
+          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>region with the word Tractor in it</t>
+          <t>The fascist council</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2378,60 +2378,60 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>239</v>
+        <v>447</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0:03:59</t>
+          <t>0:07:27</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>358</v>
+        <v>670</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0:05:58</t>
+          <t>0:11:10</t>
         </is>
       </c>
       <c r="G48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
+          <t>https://www.nationstates.net/region=the_fascist_council</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>The Kaiserreich</t>
+          <t>The Popptart Empire</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>243</v>
+        <v>469</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0:04:03</t>
+          <t>0:07:49</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>365</v>
+        <v>704</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0:06:05</t>
+          <t>0:11:44</t>
         </is>
       </c>
       <c r="G49" t="b">
@@ -2439,40 +2439,40 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kaiserreich</t>
+          <t>https://www.nationstates.net/region=the_popptart_empire</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>Ijaka, Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>The Grand British Union</t>
+          <t>Aerope</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>251</v>
+        <v>1158</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0:04:11</t>
+          <t>0:19:18</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>377</v>
+        <v>1738</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0:06:17</t>
+          <t>0:28:58</t>
         </is>
       </c>
       <c r="G50" t="b">
@@ -2480,40 +2480,40 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_grand_british_union</t>
+          <t>https://www.nationstates.net/region=aerope</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Federation of Canada</t>
+          <t>BallsMoment</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>258</v>
+        <v>1165</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0:04:18</t>
+          <t>0:19:25</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>387</v>
+        <v>1747</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0:06:27</t>
+          <t>0:29:07</t>
         </is>
       </c>
       <c r="G51" t="b">
@@ -2521,19 +2521,19 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=federation_of_canada</t>
+          <t>https://www.nationstates.net/region=ballsmoment</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>BoM, Osiris</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Card2063</t>
+          <t>Kyorgia puppet storage</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2542,19 +2542,19 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>309</v>
+        <v>1167</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0:05:09</t>
+          <t>0:19:27</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>464</v>
+        <v>1750</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0:07:44</t>
+          <t>0:29:10</t>
         </is>
       </c>
       <c r="G52" t="b">
@@ -2562,40 +2562,40 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=card2063</t>
+          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>EPSA, Lily, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>The west germanic provinces</t>
+          <t>Volantis</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>311</v>
+        <v>1175</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0:05:11</t>
+          <t>0:19:35</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>466</v>
+        <v>1762</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0:07:46</t>
+          <t>0:29:22</t>
         </is>
       </c>
       <c r="G53" t="b">
@@ -2603,40 +2603,40 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
+          <t>https://www.nationstates.net/region=volantis</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Lily, TBH</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Subaquatic</t>
+          <t>Sus amoungus</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>311</v>
+        <v>1175</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0:05:11</t>
+          <t>0:19:35</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>467</v>
+        <v>1762</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0:07:47</t>
+          <t>0:29:22</t>
         </is>
       </c>
       <c r="G54" t="b">
@@ -2644,40 +2644,40 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=subaquatic</t>
+          <t>https://www.nationstates.net/region=sus_amoungus</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Coral Reef 9</t>
+          <t>The Brotherhood of Blood</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>319</v>
+        <v>1178</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0:05:19</t>
+          <t>0:19:38</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>479</v>
+        <v>1767</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0:07:59</t>
+          <t>0:29:27</t>
         </is>
       </c>
       <c r="G55" t="b">
@@ -2685,19 +2685,19 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=coral_reef_9</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>abstrusely</t>
+          <t>NVIDIA GeForce</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2706,19 +2706,19 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>326</v>
+        <v>1179</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0:05:26</t>
+          <t>0:19:39</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>488</v>
+        <v>1768</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0:08:08</t>
+          <t>0:29:28</t>
         </is>
       </c>
       <c r="G56" t="b">
@@ -2726,40 +2726,40 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=abstrusely</t>
+          <t>https://www.nationstates.net/region=nvidia_geforce</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Freakland and Co</t>
+          <t>Stellar Crystal Tavern</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>326</v>
+        <v>1287</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0:05:26</t>
+          <t>0:21:27</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>488</v>
+        <v>1931</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0:08:08</t>
+          <t>0:32:11</t>
         </is>
       </c>
       <c r="G57" t="b">
@@ -2767,19 +2767,19 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=freakland_and_co</t>
+          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Commonwealth of Diverse Nations</t>
+          <t>The Kibble Kingdom</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2788,19 +2788,19 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>363</v>
+        <v>1813</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0:06:03</t>
+          <t>0:30:13</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>544</v>
+        <v>2719</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0:09:04</t>
+          <t>0:45:19</t>
         </is>
       </c>
       <c r="G58" t="b">
@@ -2808,40 +2808,40 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
+          <t>https://www.nationstates.net/region=the_kibble_kingdom</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>The Great States of Fascist Nudists</t>
+          <t>Regional Officers</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>489</v>
+        <v>1943</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0:08:09</t>
+          <t>0:32:23</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>733</v>
+        <v>2914</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0:12:13</t>
+          <t>0:48:34</t>
         </is>
       </c>
       <c r="G59" t="b">
@@ -2849,19 +2849,19 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
+          <t>https://www.nationstates.net/region=regional_officers</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>The fascist council</t>
+          <t>The Brotherhood of Malice Girl Scouts</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2870,19 +2870,19 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>492</v>
+        <v>2272</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0:08:12</t>
+          <t>0:37:52</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>738</v>
+        <v>3409</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0:12:18</t>
+          <t>0:56:49</t>
         </is>
       </c>
       <c r="G60" t="b">
@@ -2890,40 +2890,40 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_fascist_council</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Peoples Front</t>
+          <t>Cretanja Queendom</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>497</v>
+        <v>2313</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0:08:17</t>
+          <t>0:38:33</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>746</v>
+        <v>3469</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0:12:26</t>
+          <t>0:57:49</t>
         </is>
       </c>
       <c r="G61" t="b">
@@ -2931,40 +2931,40 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=peoples_front</t>
+          <t>https://www.nationstates.net/region=cretanja_queendom</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Fantastic</t>
+          <t>The Collective</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>504</v>
+        <v>2318</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0:08:24</t>
+          <t>0:38:38</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>756</v>
+        <v>3476</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0:12:36</t>
+          <t>0:57:56</t>
         </is>
       </c>
       <c r="G62" t="b">
@@ -2972,40 +2972,40 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=fantastic</t>
+          <t>https://www.nationstates.net/region=the_collective</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Osiris, Sparkalia, TBH</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>The Popptart Empire</t>
+          <t>Malphe</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>518</v>
+        <v>2647</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0:08:38</t>
+          <t>0:44:07</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>776</v>
+        <v>3971</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>0:12:56</t>
+          <t>1:06:11</t>
         </is>
       </c>
       <c r="G63" t="b">
@@ -3013,19 +3013,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_popptart_empire</t>
+          <t>https://www.nationstates.net/region=malphe</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>Lily, Osiris</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Greater Tyrannyistan</t>
+          <t>Violet Irises</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3034,60 +3034,60 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1025</v>
+        <v>2667</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0:17:05</t>
+          <t>0:44:27</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1537</v>
+        <v>4001</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>0:25:37</t>
+          <t>1:06:41</t>
         </is>
       </c>
       <c r="G64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=greater_tyrannyistan</t>
+          <t>https://www.nationstates.net/region=violet_irises</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Aerope</t>
+          <t>Submissive and Raidable</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1244</v>
+        <v>2855</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0:20:44</t>
+          <t>0:47:35</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1865</v>
+        <v>4282</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>0:31:05</t>
+          <t>1:11:22</t>
         </is>
       </c>
       <c r="G65" t="b">
@@ -3095,40 +3095,40 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=aerope</t>
+          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>BallsMoment</t>
+          <t>Eastern American Union</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1248</v>
+        <v>2903</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0:20:48</t>
+          <t>0:48:23</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1871</v>
+        <v>4355</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0:31:11</t>
+          <t>1:12:35</t>
         </is>
       </c>
       <c r="G66" t="b">
@@ -3136,19 +3136,19 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ballsmoment</t>
+          <t>https://www.nationstates.net/region=eastern_american_union</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>BoM, Osiris</t>
+          <t>Lily, TBH</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Kyorgia puppet storage</t>
+          <t>The beforelife</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3157,19 +3157,19 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1250</v>
+        <v>2942</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>0:20:50</t>
+          <t>0:49:02</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1874</v>
+        <v>4413</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>0:31:14</t>
+          <t>1:13:33</t>
         </is>
       </c>
       <c r="G67" t="b">
@@ -3177,19 +3177,19 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
+          <t>https://www.nationstates.net/region=the_beforelife</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>EPSA, Lily, Osiris, TBH</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>The Empire Of The Magisterium</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3198,19 +3198,19 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1252</v>
+        <v>3138</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0:20:52</t>
+          <t>0:52:18</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>1879</v>
+        <v>4707</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0:31:19</t>
+          <t>1:18:27</t>
         </is>
       </c>
       <c r="G68" t="b">
@@ -3218,40 +3218,40 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_empire_of_the_magisterium</t>
+          <t>https://www.nationstates.net/region=ben</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Agia Germania Anest</t>
+          <t>Brest Oblast</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1253</v>
+        <v>3341</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0:20:53</t>
+          <t>0:55:41</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1880</v>
+        <v>5012</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>0:31:20</t>
+          <t>1:23:32</t>
         </is>
       </c>
       <c r="G69" t="b">
@@ -3259,789 +3259,10 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=agia_germania_anest</t>
+          <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
-        <is>
-          <t>Lily</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Volantis</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>WFE, Embassies</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>1256</v>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>0:20:56</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>1884</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>0:31:24</t>
-        </is>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=volantis</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>Lily, TBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Sus amoungus</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>RO</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
-        <v>1256</v>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>0:20:56</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>1885</v>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>0:31:25</t>
-        </is>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=sus_amoungus</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>Lily</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>The Brotherhood of Blood</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>RO</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>1260</v>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>0:21:00</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>1890</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>0:31:30</t>
-        </is>
-      </c>
-      <c r="G72" t="b">
-        <v>0</v>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>NVIDIA GeForce</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>RO</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>1260</v>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>0:21:00</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>1890</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>0:31:30</t>
-        </is>
-      </c>
-      <c r="G73" t="b">
-        <v>0</v>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=nvidia_geforce</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Stellar Crystal Tavern</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>1350</v>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>0:22:30</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>0:33:45</t>
-        </is>
-      </c>
-      <c r="G74" t="b">
-        <v>0</v>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>Osiris, TBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>The Kibble Kingdom</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>1864</v>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>0:31:04</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>2796</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>0:46:36</t>
-        </is>
-      </c>
-      <c r="G75" t="b">
-        <v>0</v>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=the_kibble_kingdom</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>TBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Regional Officers</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C76" t="n">
-        <v>1978</v>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>0:32:58</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
-        <v>2966</v>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>0:49:26</t>
-        </is>
-      </c>
-      <c r="G76" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=regional_officers</t>
-        </is>
-      </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>TCB</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Slavya</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>WFE, Embassies</t>
-        </is>
-      </c>
-      <c r="C77" t="n">
-        <v>1985</v>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>0:33:05</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>2978</v>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>0:49:38</t>
-        </is>
-      </c>
-      <c r="G77" t="b">
-        <v>0</v>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=slavya</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>Ijaka, Sparkalia</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Nonglefungliodlia</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C78" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>0:33:43</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>3034</v>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>0:50:34</t>
-        </is>
-      </c>
-      <c r="G78" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=nonglefungliodlia</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>Sparkalia</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>The Brotherhood of Malice Girl Scouts</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C79" t="n">
-        <v>2332</v>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>0:38:52</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>3498</v>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>0:58:18</t>
-        </is>
-      </c>
-      <c r="G79" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>BoM</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Cretanja Queendom</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
-        <v>2373</v>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>0:39:33</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>3560</v>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>0:59:20</t>
-        </is>
-      </c>
-      <c r="G80" t="b">
-        <v>0</v>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=cretanja_queendom</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>Osiris</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>The Collective</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>WFE</t>
-        </is>
-      </c>
-      <c r="C81" t="n">
-        <v>2378</v>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>0:39:38</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>3567</v>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>0:59:27</t>
-        </is>
-      </c>
-      <c r="G81" t="b">
-        <v>0</v>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=the_collective</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>Lily</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Malphe</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C82" t="n">
-        <v>2688</v>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>0:44:48</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>4032</v>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>1:07:12</t>
-        </is>
-      </c>
-      <c r="G82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=malphe</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>Lily, Osiris</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Violet Irises</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C83" t="n">
-        <v>2703</v>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>0:45:03</t>
-        </is>
-      </c>
-      <c r="E83" t="n">
-        <v>4054</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>1:07:34</t>
-        </is>
-      </c>
-      <c r="G83" t="b">
-        <v>0</v>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=violet_irises</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>TBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>Submissive and Raidable</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>WFE</t>
-        </is>
-      </c>
-      <c r="C84" t="n">
-        <v>2903</v>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>0:48:23</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
-        <v>4355</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>1:12:35</t>
-        </is>
-      </c>
-      <c r="G84" t="b">
-        <v>0</v>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>BoM</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>Eastern American Union</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>WFE</t>
-        </is>
-      </c>
-      <c r="C85" t="n">
-        <v>2952</v>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>0:49:12</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
-        <v>4427</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>1:13:47</t>
-        </is>
-      </c>
-      <c r="G85" t="b">
-        <v>0</v>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=eastern_american_union</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>Lily, TBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>The beforelife</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C86" t="n">
-        <v>2991</v>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>0:49:51</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
-        <v>4486</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>1:14:46</t>
-        </is>
-      </c>
-      <c r="G86" t="b">
-        <v>0</v>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=the_beforelife</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>Ijaka</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>Ben</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C87" t="n">
-        <v>3185</v>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>0:53:05</t>
-        </is>
-      </c>
-      <c r="E87" t="n">
-        <v>4777</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>1:19:37</t>
-        </is>
-      </c>
-      <c r="G87" t="b">
-        <v>0</v>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=ben</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>Osiris</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>Brest Oblast</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C88" t="n">
-        <v>3385</v>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>0:56:25</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
-        <v>5077</v>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>1:24:37</t>
-        </is>
-      </c>
-      <c r="G88" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=brest_oblast</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Fix practice detag flagging
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="30 March 2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="31 March 2023" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,19 +492,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0:01:09</t>
+          <t>0:01:21</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:01:44</t>
+          <t>0:02:01</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0:01:11</t>
+          <t>0:01:21</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0:01:46</t>
+          <t>0:02:02</t>
         </is>
       </c>
       <c r="G3" t="b">
@@ -574,19 +574,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0:01:15</t>
+          <t>0:01:26</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:01:52</t>
+          <t>0:02:09</t>
         </is>
       </c>
       <c r="G4" t="b">
@@ -615,19 +615,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0:01:15</t>
+          <t>0:01:27</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:01:53</t>
+          <t>0:02:10</t>
         </is>
       </c>
       <c r="G5" t="b">
@@ -656,19 +656,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0:01:15</t>
+          <t>0:01:27</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:01:53</t>
+          <t>0:02:10</t>
         </is>
       </c>
       <c r="G6" t="b">
@@ -697,19 +697,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0:01:24</t>
+          <t>0:01:40</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:02:06</t>
+          <t>0:02:30</t>
         </is>
       </c>
       <c r="G7" t="b">
@@ -738,19 +738,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0:01:34</t>
+          <t>0:01:49</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:02:22</t>
+          <t>0:02:43</t>
         </is>
       </c>
       <c r="G8" t="b">
@@ -779,19 +779,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0:01:38</t>
+          <t>0:01:52</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:02:28</t>
+          <t>0:02:48</t>
         </is>
       </c>
       <c r="G9" t="b">
@@ -820,19 +820,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0:01:40</t>
+          <t>0:01:58</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:02:30</t>
+          <t>0:02:57</t>
         </is>
       </c>
       <c r="G10" t="b">
@@ -861,19 +861,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0:01:40</t>
+          <t>0:01:58</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:02:30</t>
+          <t>0:02:57</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0:01:40</t>
+          <t>0:01:58</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:02:30</t>
+          <t>0:02:57</t>
         </is>
       </c>
       <c r="G12" t="b">
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0:01:40</t>
+          <t>0:01:59</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:02:30</t>
+          <t>0:02:58</t>
         </is>
       </c>
       <c r="G13" t="b">
@@ -975,28 +975,28 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>The Democratic Group Of Asia</t>
+          <t>Dragonborn Confederate</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0:01:42</t>
+          <t>0:02:02</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:02:33</t>
+          <t>0:03:04</t>
         </is>
       </c>
       <c r="G14" t="b">
@@ -1004,40 +1004,40 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_democratic_group_of_asia</t>
+          <t>https://www.nationstates.net/region=dragonborn_confederate</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Dragonborn Confederate</t>
+          <t>The Confederacy of German States</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0:01:42</t>
+          <t>0:02:02</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:02:34</t>
+          <t>0:03:04</t>
         </is>
       </c>
       <c r="G15" t="b">
@@ -1045,40 +1045,40 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=dragonborn_confederate</t>
+          <t>https://www.nationstates.net/region=the_confederacy_of_german_states</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>The Confederacy of German States</t>
+          <t>Solar Union</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0:01:42</t>
+          <t>0:02:03</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:02:34</t>
+          <t>0:03:05</t>
         </is>
       </c>
       <c r="G16" t="b">
@@ -1086,40 +1086,40 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_confederacy_of_german_states</t>
+          <t>https://www.nationstates.net/region=solar_union</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Solar Union</t>
+          <t>Yusmoydal</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0:01:43</t>
+          <t>0:02:18</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:02:35</t>
+          <t>0:03:28</t>
         </is>
       </c>
       <c r="G17" t="b">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=solar_union</t>
+          <t>https://www.nationstates.net/region=yusmoydal</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1139,7 +1139,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Yusmoydal</t>
+          <t>The gamma quadrant</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1148,19 +1148,19 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0:01:57</t>
+          <t>0:02:19</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0:02:55</t>
+          <t>0:03:29</t>
         </is>
       </c>
       <c r="G18" t="b">
@@ -1168,40 +1168,40 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=yusmoydal</t>
+          <t>https://www.nationstates.net/region=the_gamma_quadrant</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>The gamma quadrant</t>
+          <t>Pride Rock</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0:01:57</t>
+          <t>0:02:22</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0:02:56</t>
+          <t>0:03:33</t>
         </is>
       </c>
       <c r="G19" t="b">
@@ -1209,40 +1209,40 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_gamma_quadrant</t>
+          <t>https://www.nationstates.net/region=pride_rock</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>ERN</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Pride Rock</t>
+          <t>The United World Region</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0:02:05</t>
+          <t>0:02:23</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0:03:07</t>
+          <t>0:03:35</t>
         </is>
       </c>
       <c r="G20" t="b">
@@ -1250,19 +1250,19 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=pride_rock</t>
+          <t>https://www.nationstates.net/region=the_united_world_region</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>ERN</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>The United World Region</t>
+          <t>Northern Ameria</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1271,19 +1271,19 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0:02:05</t>
+          <t>0:02:27</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0:03:08</t>
+          <t>0:03:41</t>
         </is>
       </c>
       <c r="G21" t="b">
@@ -1291,40 +1291,40 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_united_world_region</t>
+          <t>https://www.nationstates.net/region=northern_ameria</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Northern Ameria</t>
+          <t>The UN Of The Universal Republic</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0:02:09</t>
+          <t>0:02:35</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>194</v>
+        <v>233</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0:03:14</t>
+          <t>0:03:53</t>
         </is>
       </c>
       <c r="G22" t="b">
@@ -1332,40 +1332,40 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=northern_ameria</t>
+          <t>https://www.nationstates.net/region=the_un_of_the_universal_republic</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>The UN Of The Universal Republic</t>
+          <t>accession</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0:02:15</t>
+          <t>0:02:35</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0:03:22</t>
+          <t>0:03:53</t>
         </is>
       </c>
       <c r="G23" t="b">
@@ -1373,40 +1373,40 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_un_of_the_universal_republic</t>
+          <t>https://www.nationstates.net/region=accession</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>BoM, Osiris</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>accession</t>
+          <t>The Jewel Robotox Nations</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0:02:15</t>
+          <t>0:02:38</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0:03:22</t>
+          <t>0:03:57</t>
         </is>
       </c>
       <c r="G24" t="b">
@@ -1414,19 +1414,19 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=accession</t>
+          <t>https://www.nationstates.net/region=the_jewel_robotox_nations</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>BoM, Osiris</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>The Jewel Robotox Nations</t>
+          <t>Budget Crackheads</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1435,19 +1435,19 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0:02:17</t>
+          <t>0:02:44</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0:03:25</t>
+          <t>0:04:06</t>
         </is>
       </c>
       <c r="G25" t="b">
@@ -1455,19 +1455,19 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_jewel_robotox_nations</t>
+          <t>https://www.nationstates.net/region=budget_crackheads</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Goth Girls United</t>
+          <t>Union of Dystopias</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1476,19 +1476,19 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0:02:19</t>
+          <t>0:02:47</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0:03:29</t>
+          <t>0:04:11</t>
         </is>
       </c>
       <c r="G26" t="b">
@@ -1496,40 +1496,40 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=goth_girls_united</t>
+          <t>https://www.nationstates.net/region=union_of_dystopias</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Sparkalia, TBH</t>
+          <t>Ijaka, Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Budget Crackheads</t>
+          <t>The Koprulu Sector</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0:02:25</t>
+          <t>0:03:00</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0:03:37</t>
+          <t>0:04:30</t>
         </is>
       </c>
       <c r="G27" t="b">
@@ -1537,40 +1537,40 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=budget_crackheads</t>
+          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Union of Dystopias</t>
+          <t>South Asian Association for Cooperation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0:02:28</t>
+          <t>0:03:02</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0:03:42</t>
+          <t>0:04:33</t>
         </is>
       </c>
       <c r="G28" t="b">
@@ -1578,40 +1578,40 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_dystopias</t>
+          <t>https://www.nationstates.net/region=south_asian_association_for_cooperation</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>The Koprulu Sector</t>
+          <t>accented</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0:02:38</t>
+          <t>0:03:12</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>237</v>
+        <v>288</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0:03:57</t>
+          <t>0:04:48</t>
         </is>
       </c>
       <c r="G29" t="b">
@@ -1619,19 +1619,19 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
+          <t>https://www.nationstates.net/region=accented</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>South Asian Association for Cooperation</t>
+          <t>The Kaisers</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1640,19 +1640,19 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0:02:39</t>
+          <t>0:03:16</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0:03:59</t>
+          <t>0:04:53</t>
         </is>
       </c>
       <c r="G30" t="b">
@@ -1660,40 +1660,40 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=south_asian_association_for_cooperation</t>
+          <t>https://www.nationstates.net/region=the_kaisers</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>accented</t>
+          <t>Polcom</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0:02:46</t>
+          <t>0:04:04</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>250</v>
+        <v>366</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0:04:10</t>
+          <t>0:06:06</t>
         </is>
       </c>
       <c r="G31" t="b">
@@ -1701,12 +1701,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=accented</t>
+          <t>https://www.nationstates.net/region=polcom</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
@@ -1722,19 +1722,19 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>193</v>
+        <v>245</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0:03:13</t>
+          <t>0:04:05</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>290</v>
+        <v>367</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0:04:50</t>
+          <t>0:06:07</t>
         </is>
       </c>
       <c r="G32" t="b">
@@ -1763,19 +1763,19 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0:03:15</t>
+          <t>0:04:09</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>293</v>
+        <v>374</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0:04:53</t>
+          <t>0:06:14</t>
         </is>
       </c>
       <c r="G33" t="b">
@@ -1804,19 +1804,19 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0:03:15</t>
+          <t>0:04:10</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>293</v>
+        <v>375</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0:04:53</t>
+          <t>0:06:15</t>
         </is>
       </c>
       <c r="G34" t="b">
@@ -1845,19 +1845,19 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0:03:16</t>
+          <t>0:04:10</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>294</v>
+        <v>375</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0:04:54</t>
+          <t>0:06:15</t>
         </is>
       </c>
       <c r="G35" t="b">
@@ -1886,19 +1886,19 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0:03:21</t>
+          <t>0:04:11</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>301</v>
+        <v>376</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0:05:01</t>
+          <t>0:06:16</t>
         </is>
       </c>
       <c r="G36" t="b">
@@ -1918,28 +1918,28 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Hukashaka</t>
+          <t>New Nortvia</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>201</v>
+        <v>255</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0:03:21</t>
+          <t>0:04:15</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>302</v>
+        <v>382</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0:05:02</t>
+          <t>0:06:22</t>
         </is>
       </c>
       <c r="G37" t="b">
@@ -1947,40 +1947,40 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=hukashaka</t>
+          <t>https://www.nationstates.net/region=new_nortvia</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>New Nortvia</t>
+          <t>Union of United Democratic States</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0:03:24</t>
+          <t>0:04:15</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>305</v>
+        <v>382</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0:05:05</t>
+          <t>0:06:22</t>
         </is>
       </c>
       <c r="G38" t="b">
@@ -1988,60 +1988,60 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=new_nortvia</t>
+          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Osiris, Sparkalia, TBH</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Union of United Democratic States</t>
+          <t>region with the word Tractor in it</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>204</v>
+        <v>258</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0:03:24</t>
+          <t>0:04:18</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>305</v>
+        <v>387</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0:05:05</t>
+          <t>0:06:27</t>
         </is>
       </c>
       <c r="G39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_united_democratic_states</t>
+          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>region with the word Tractor in it</t>
+          <t>The Kaiserreich</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2050,60 +2050,60 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0:03:44</t>
+          <t>0:04:24</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>337</v>
+        <v>395</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0:05:37</t>
+          <t>0:06:35</t>
         </is>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
+          <t>https://www.nationstates.net/region=the_kaiserreich</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>The Kaiserreich</t>
+          <t>The west germanic provinces</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>228</v>
+        <v>332</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0:03:48</t>
+          <t>0:05:32</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>343</v>
+        <v>498</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0:05:43</t>
+          <t>0:08:18</t>
         </is>
       </c>
       <c r="G41" t="b">
@@ -2111,40 +2111,40 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kaiserreich</t>
+          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>The west germanic provinces</t>
+          <t>Subaquatic</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>295</v>
+        <v>333</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0:04:55</t>
+          <t>0:05:33</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>443</v>
+        <v>499</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0:07:23</t>
+          <t>0:08:19</t>
         </is>
       </c>
       <c r="G42" t="b">
@@ -2152,40 +2152,40 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
+          <t>https://www.nationstates.net/region=subaquatic</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Subaquatic</t>
+          <t>abstrusely</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>297</v>
+        <v>343</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0:04:57</t>
+          <t>0:05:43</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>446</v>
+        <v>514</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0:07:26</t>
+          <t>0:08:34</t>
         </is>
       </c>
       <c r="G43" t="b">
@@ -2193,19 +2193,19 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=subaquatic</t>
+          <t>https://www.nationstates.net/region=abstrusely</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>abstrusely</t>
+          <t>Freakland and Co</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2214,19 +2214,19 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0:05:05</t>
+          <t>0:05:44</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>458</v>
+        <v>515</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0:07:38</t>
+          <t>0:08:35</t>
         </is>
       </c>
       <c r="G44" t="b">
@@ -2234,40 +2234,40 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=abstrusely</t>
+          <t>https://www.nationstates.net/region=freakland_and_co</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Freakland and Co</t>
+          <t>Commonwealth of Diverse Nations</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>305</v>
+        <v>374</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0:05:05</t>
+          <t>0:06:14</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>458</v>
+        <v>561</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0:07:38</t>
+          <t>0:09:21</t>
         </is>
       </c>
       <c r="G45" t="b">
@@ -2275,40 +2275,40 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=freakland_and_co</t>
+          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Commonwealth of Diverse Nations</t>
+          <t>The Great States of Fascist Nudists</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>330</v>
+        <v>538</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0:05:30</t>
+          <t>0:08:58</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>495</v>
+        <v>808</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0:08:15</t>
+          <t>0:13:28</t>
         </is>
       </c>
       <c r="G46" t="b">
@@ -2316,40 +2316,40 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
+          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>The Great States of Fascist Nudists</t>
+          <t>The fascist council</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>443</v>
+        <v>549</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0:07:23</t>
+          <t>0:09:09</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>665</v>
+        <v>823</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0:11:05</t>
+          <t>0:13:43</t>
         </is>
       </c>
       <c r="G47" t="b">
@@ -2357,40 +2357,40 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
+          <t>https://www.nationstates.net/region=the_fascist_council</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>The fascist council</t>
+          <t>The Popptart Empire</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>447</v>
+        <v>574</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0:07:27</t>
+          <t>0:09:34</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0:11:10</t>
+          <t>0:14:21</t>
         </is>
       </c>
       <c r="G48" t="b">
@@ -2398,60 +2398,60 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_fascist_council</t>
+          <t>https://www.nationstates.net/region=the_popptart_empire</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>Ijaka, Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>The Popptart Empire</t>
+          <t>Greater Tyrannyistan</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>469</v>
+        <v>1088</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0:07:49</t>
+          <t>0:18:08</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>704</v>
+        <v>1633</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0:11:44</t>
+          <t>0:27:13</t>
         </is>
       </c>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_popptart_empire</t>
+          <t>https://www.nationstates.net/region=greater_tyrannyistan</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Ijaka, Sparkalia</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Aerope</t>
+          <t>Za Za garden</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2460,19 +2460,19 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1158</v>
+        <v>1273</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0:19:18</t>
+          <t>0:21:13</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>1738</v>
+        <v>1910</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0:28:58</t>
+          <t>0:31:50</t>
         </is>
       </c>
       <c r="G50" t="b">
@@ -2480,40 +2480,40 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=aerope</t>
+          <t>https://www.nationstates.net/region=za_za_garden</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>BallsMoment</t>
+          <t>Aerope</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1165</v>
+        <v>1289</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0:19:25</t>
+          <t>0:21:29</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>1747</v>
+        <v>1934</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0:29:07</t>
+          <t>0:32:14</t>
         </is>
       </c>
       <c r="G51" t="b">
@@ -2521,40 +2521,40 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ballsmoment</t>
+          <t>https://www.nationstates.net/region=aerope</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>BoM, Osiris</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Kyorgia puppet storage</t>
+          <t>BallsMoment</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1167</v>
+        <v>1293</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0:19:27</t>
+          <t>0:21:33</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1750</v>
+        <v>1939</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0:29:10</t>
+          <t>0:32:19</t>
         </is>
       </c>
       <c r="G52" t="b">
@@ -2562,40 +2562,40 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
+          <t>https://www.nationstates.net/region=ballsmoment</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>EPSA, Lily, Osiris, TBH</t>
+          <t>BoM, Osiris</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Volantis</t>
+          <t>Kyorgia puppet storage</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1175</v>
+        <v>1294</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0:19:35</t>
+          <t>0:21:34</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1762</v>
+        <v>1941</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0:29:22</t>
+          <t>0:32:21</t>
         </is>
       </c>
       <c r="G53" t="b">
@@ -2603,40 +2603,40 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=volantis</t>
+          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>EPSA, Lily, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Sus amoungus</t>
+          <t>Volantis</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1175</v>
+        <v>1300</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0:19:35</t>
+          <t>0:21:40</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1762</v>
+        <v>1950</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0:29:22</t>
+          <t>0:32:30</t>
         </is>
       </c>
       <c r="G54" t="b">
@@ -2644,19 +2644,19 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=sus_amoungus</t>
+          <t>https://www.nationstates.net/region=volantis</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Lily, TBH</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Blood</t>
+          <t>Sus amoungus</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2665,19 +2665,19 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1178</v>
+        <v>1301</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0:19:38</t>
+          <t>0:21:41</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1767</v>
+        <v>1951</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0:29:27</t>
+          <t>0:32:31</t>
         </is>
       </c>
       <c r="G55" t="b">
@@ -2685,19 +2685,19 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
+          <t>https://www.nationstates.net/region=sus_amoungus</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>NVIDIA GeForce</t>
+          <t>The Brotherhood of Blood</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2706,19 +2706,19 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1179</v>
+        <v>1305</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0:19:39</t>
+          <t>0:21:45</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1768</v>
+        <v>1957</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0:29:28</t>
+          <t>0:32:37</t>
         </is>
       </c>
       <c r="G56" t="b">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=nvidia_geforce</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2738,28 +2738,28 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Stellar Crystal Tavern</t>
+          <t>NVIDIA GeForce</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1287</v>
+        <v>1305</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0:21:27</t>
+          <t>0:21:45</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>1931</v>
+        <v>1957</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0:32:11</t>
+          <t>0:32:37</t>
         </is>
       </c>
       <c r="G57" t="b">
@@ -2767,19 +2767,19 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
+          <t>https://www.nationstates.net/region=nvidia_geforce</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Osiris, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>The Kibble Kingdom</t>
+          <t>Stellar Crystal Tavern</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2788,19 +2788,19 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1813</v>
+        <v>1384</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0:30:13</t>
+          <t>0:23:04</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>2719</v>
+        <v>2076</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0:45:19</t>
+          <t>0:34:36</t>
         </is>
       </c>
       <c r="G58" t="b">
@@ -2808,19 +2808,19 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_kibble_kingdom</t>
+          <t>https://www.nationstates.net/region=stellar_crystal_tavern</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Regional Officers</t>
+          <t>zenya</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2829,19 +2829,19 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1943</v>
+        <v>1474</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0:32:23</t>
+          <t>0:24:34</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2914</v>
+        <v>2211</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0:48:34</t>
+          <t>0:36:51</t>
         </is>
       </c>
       <c r="G59" t="b">
@@ -2849,19 +2849,19 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=regional_officers</t>
+          <t>https://www.nationstates.net/region=zenya</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Malice Girl Scouts</t>
+          <t>Regional Officers</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2870,19 +2870,19 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2272</v>
+        <v>1946</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0:37:52</t>
+          <t>0:32:26</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>3409</v>
+        <v>2919</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0:56:49</t>
+          <t>0:48:39</t>
         </is>
       </c>
       <c r="G60" t="b">
@@ -2890,19 +2890,19 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
+          <t>https://www.nationstates.net/region=regional_officers</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Cretanja Queendom</t>
+          <t>The Brotherhood of Malice Girl Scouts</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2911,19 +2911,19 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2313</v>
+        <v>2275</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0:38:33</t>
+          <t>0:37:55</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>3469</v>
+        <v>3412</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0:57:49</t>
+          <t>0:56:52</t>
         </is>
       </c>
       <c r="G61" t="b">
@@ -2931,40 +2931,40 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cretanja_queendom</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>The Collective</t>
+          <t>Cretanja Queendom</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2318</v>
+        <v>2312</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0:38:38</t>
+          <t>0:38:32</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>3476</v>
+        <v>3468</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0:57:56</t>
+          <t>0:57:48</t>
         </is>
       </c>
       <c r="G62" t="b">
@@ -2972,40 +2972,40 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_collective</t>
+          <t>https://www.nationstates.net/region=cretanja_queendom</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Malphe</t>
+          <t>The Collective</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2647</v>
+        <v>2316</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0:44:07</t>
+          <t>0:38:36</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>3971</v>
+        <v>3474</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>1:06:11</t>
+          <t>0:57:54</t>
         </is>
       </c>
       <c r="G63" t="b">
@@ -3013,19 +3013,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=malphe</t>
+          <t>https://www.nationstates.net/region=the_collective</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Lily, Osiris</t>
+          <t>Lily</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Violet Irises</t>
+          <t>Malphe</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3034,19 +3034,19 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2667</v>
+        <v>2647</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0:44:27</t>
+          <t>0:44:07</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>4001</v>
+        <v>3971</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>1:06:41</t>
+          <t>1:06:11</t>
         </is>
       </c>
       <c r="G64" t="b">
@@ -3054,40 +3054,40 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=violet_irises</t>
+          <t>https://www.nationstates.net/region=malphe</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Lily, Osiris</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Submissive and Raidable</t>
+          <t>Violet Irises</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2855</v>
+        <v>2662</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0:47:35</t>
+          <t>0:44:22</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>4282</v>
+        <v>3993</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>1:11:22</t>
+          <t>1:06:33</t>
         </is>
       </c>
       <c r="G65" t="b">
@@ -3095,19 +3095,19 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+          <t>https://www.nationstates.net/region=violet_irises</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Eastern American Union</t>
+          <t>Submissive and Raidable</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3116,19 +3116,19 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2903</v>
+        <v>2846</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0:48:23</t>
+          <t>0:47:26</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>4355</v>
+        <v>4270</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>1:12:35</t>
+          <t>1:11:10</t>
         </is>
       </c>
       <c r="G66" t="b">
@@ -3136,40 +3136,40 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=eastern_american_union</t>
+          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>The beforelife</t>
+          <t>Eastern American Union</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2942</v>
+        <v>2894</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>0:49:02</t>
+          <t>0:48:14</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>4413</v>
+        <v>4341</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>1:13:33</t>
+          <t>1:12:21</t>
         </is>
       </c>
       <c r="G67" t="b">
@@ -3177,19 +3177,19 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_beforelife</t>
+          <t>https://www.nationstates.net/region=eastern_american_union</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Lily, TBH</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>The beforelife</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3198,19 +3198,19 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3138</v>
+        <v>2929</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0:52:18</t>
+          <t>0:48:49</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>4707</v>
+        <v>4394</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>1:18:27</t>
+          <t>1:13:14</t>
         </is>
       </c>
       <c r="G68" t="b">
@@ -3218,51 +3218,92 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ben</t>
+          <t>https://www.nationstates.net/region=the_beforelife</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>Ijaka</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3123</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0:52:03</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>4684</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>1:18:04</t>
+        </is>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=ben</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
           <t>Brest Oblast</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>Embassies</t>
         </is>
       </c>
-      <c r="C69" t="n">
-        <v>3341</v>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>0:55:41</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
-        <v>5012</v>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>1:23:32</t>
-        </is>
-      </c>
-      <c r="G69" t="b">
-        <v>0</v>
-      </c>
-      <c r="H69" t="inlineStr">
+      <c r="C70" t="n">
+        <v>3353</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0:55:53</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>5030</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1:23:50</t>
+        </is>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="inlineStr">
         <is>
           <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr">
+      <c r="I70" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Exclude denied embassy requests
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3189,7 +3189,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>The beforelife</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3198,19 +3198,19 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2929</v>
+        <v>3123</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0:48:49</t>
+          <t>0:52:03</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>4394</v>
+        <v>4684</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>1:13:14</t>
+          <t>1:18:04</t>
         </is>
       </c>
       <c r="G68" t="b">
@@ -3218,19 +3218,19 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_beforelife</t>
+          <t>https://www.nationstates.net/region=ben</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Ijaka</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Brest Oblast</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3239,19 +3239,19 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3123</v>
+        <v>3353</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0:52:03</t>
+          <t>0:55:53</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>4684</v>
+        <v>5030</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>1:18:04</t>
+          <t>1:23:50</t>
         </is>
       </c>
       <c r="G69" t="b">
@@ -3259,51 +3259,10 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ben</t>
+          <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
-        <is>
-          <t>Osiris</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Brest Oblast</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Embassies</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>3353</v>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>0:55:53</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>5030</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>1:23:50</t>
-        </is>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>https://www.nationstates.net/region=brest_oblast</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Flag NPA and BFL tags
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1262,28 +1262,28 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Bakayatist Region</t>
+          <t>The League of Free Nations</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0:08:15</t>
+          <t>0:08:10</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0:12:22</t>
+          <t>0:12:15</t>
         </is>
       </c>
       <c r="G21" t="b">
@@ -1291,40 +1291,40 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=bakayatist_region</t>
+          <t>https://www.nationstates.net/region=the_league_of_free_nations</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>NPA</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>The Great States of Fascist Nudists</t>
+          <t>Bakayatist Region</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0:08:19</t>
+          <t>0:08:15</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0:12:28</t>
+          <t>0:12:22</t>
         </is>
       </c>
       <c r="G22" t="b">
@@ -1332,40 +1332,40 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
+          <t>https://www.nationstates.net/region=bakayatist_region</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>absolves</t>
+          <t>The Great States of Fascist Nudists</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>676</v>
+        <v>499</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0:11:16</t>
+          <t>0:08:19</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1014</v>
+        <v>748</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0:16:54</t>
+          <t>0:12:28</t>
         </is>
       </c>
       <c r="G23" t="b">
@@ -1373,40 +1373,40 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=absolves</t>
+          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Confederate Nations of TomFoolery</t>
+          <t>The Socialist Countries</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>760</v>
+        <v>674</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0:12:40</t>
+          <t>0:11:14</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1141</v>
+        <v>1011</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0:19:01</t>
+          <t>0:16:51</t>
         </is>
       </c>
       <c r="G24" t="b">
@@ -1414,40 +1414,40 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=confederate_nations_of_tomfoolery</t>
+          <t>https://www.nationstates.net/region=the_socialist_countries</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>BFL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Ooftopia</t>
+          <t>absolves</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>777</v>
+        <v>676</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0:12:57</t>
+          <t>0:11:16</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1166</v>
+        <v>1014</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0:19:26</t>
+          <t>0:16:54</t>
         </is>
       </c>
       <c r="G25" t="b">
@@ -1455,19 +1455,19 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=ooftopia</t>
+          <t>https://www.nationstates.net/region=absolves</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>LIFE PUPPETS</t>
+          <t>Confederate Nations of TomFoolery</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1476,19 +1476,19 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>797</v>
+        <v>760</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0:13:17</t>
+          <t>0:12:40</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1195</v>
+        <v>1141</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0:19:55</t>
+          <t>0:19:01</t>
         </is>
       </c>
       <c r="G26" t="b">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=life_puppets</t>
+          <t>https://www.nationstates.net/region=confederate_nations_of_tomfoolery</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>atlantiantic</t>
+          <t>Ooftopia</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1517,19 +1517,19 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>834</v>
+        <v>777</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0:13:54</t>
+          <t>0:12:57</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1251</v>
+        <v>1166</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0:20:51</t>
+          <t>0:19:26</t>
         </is>
       </c>
       <c r="G27" t="b">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=atlantiantic</t>
+          <t>https://www.nationstates.net/region=ooftopia</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1549,7 +1549,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Huago</t>
+          <t>LIFE PUPPETS</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1558,19 +1558,19 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>888</v>
+        <v>797</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0:14:48</t>
+          <t>0:13:17</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1332</v>
+        <v>1195</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0:22:12</t>
+          <t>0:19:55</t>
         </is>
       </c>
       <c r="G28" t="b">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=huago</t>
+          <t>https://www.nationstates.net/region=life_puppets</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1590,7 +1590,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Cicimboroughian Coalition</t>
+          <t>atlantiantic</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1599,19 +1599,19 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1041</v>
+        <v>834</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0:17:21</t>
+          <t>0:13:54</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1561</v>
+        <v>1251</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0:26:01</t>
+          <t>0:20:51</t>
         </is>
       </c>
       <c r="G29" t="b">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cicimboroughian_coalition</t>
+          <t>https://www.nationstates.net/region=atlantiantic</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1631,7 +1631,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Mojave Wasteland</t>
+          <t>Huago</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1640,19 +1640,19 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1078</v>
+        <v>888</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0:17:58</t>
+          <t>0:14:48</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1618</v>
+        <v>1332</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0:26:58</t>
+          <t>0:22:12</t>
         </is>
       </c>
       <c r="G30" t="b">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=mojave_wasteland</t>
+          <t>https://www.nationstates.net/region=huago</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1672,28 +1672,28 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Aerope</t>
+          <t>New Vegas</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1215</v>
+        <v>1039</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0:20:15</t>
+          <t>0:17:19</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1822</v>
+        <v>1559</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0:30:22</t>
+          <t>0:25:59</t>
         </is>
       </c>
       <c r="G31" t="b">
@@ -1701,40 +1701,40 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=aerope</t>
+          <t>https://www.nationstates.net/region=new_vegas</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>NPA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Kyorgia puppet storage</t>
+          <t>Cicimboroughian Coalition</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1220</v>
+        <v>1041</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0:20:20</t>
+          <t>0:17:21</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1830</v>
+        <v>1561</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0:30:30</t>
+          <t>0:26:01</t>
         </is>
       </c>
       <c r="G32" t="b">
@@ -1742,19 +1742,19 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
+          <t>https://www.nationstates.net/region=cicimboroughian_coalition</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>EPSA, Lily, Osiris, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Blood</t>
+          <t>Mojave Wasteland</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1763,19 +1763,19 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1231</v>
+        <v>1078</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0:20:31</t>
+          <t>0:17:58</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1847</v>
+        <v>1618</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0:30:47</t>
+          <t>0:26:58</t>
         </is>
       </c>
       <c r="G33" t="b">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
+          <t>https://www.nationstates.net/region=mojave_wasteland</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1795,28 +1795,28 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Tropical Islands</t>
+          <t>Aerope</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1234</v>
+        <v>1215</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0:20:34</t>
+          <t>0:20:15</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1851</v>
+        <v>1822</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0:30:51</t>
+          <t>0:30:22</t>
         </is>
       </c>
       <c r="G34" t="b">
@@ -1824,40 +1824,40 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=tropical_islands</t>
+          <t>https://www.nationstates.net/region=aerope</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>The Federation of the FA</t>
+          <t>Kyorgia puppet storage</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1359</v>
+        <v>1220</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0:22:39</t>
+          <t>0:20:20</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2039</v>
+        <v>1830</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0:33:59</t>
+          <t>0:30:30</t>
         </is>
       </c>
       <c r="G35" t="b">
@@ -1865,40 +1865,40 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_federation_of_the_fa</t>
+          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>EPSA, Lily, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>The Westerlands</t>
+          <t>Nizhyn</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1425</v>
+        <v>1229</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0:23:45</t>
+          <t>0:20:29</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2137</v>
+        <v>1844</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0:35:37</t>
+          <t>0:30:44</t>
         </is>
       </c>
       <c r="G36" t="b">
@@ -1906,40 +1906,40 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_westerlands</t>
+          <t>https://www.nationstates.net/region=nizhyn</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>BFL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>The Region of Peace</t>
+          <t>The Brotherhood of Blood</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1502</v>
+        <v>1231</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0:25:02</t>
+          <t>0:20:31</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2253</v>
+        <v>1847</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0:37:33</t>
+          <t>0:30:47</t>
         </is>
       </c>
       <c r="G37" t="b">
@@ -1947,40 +1947,40 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_region_of_peace</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Too</t>
+          <t>Tropical Islands</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1631</v>
+        <v>1234</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0:27:11</t>
+          <t>0:20:34</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2447</v>
+        <v>1851</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0:40:47</t>
+          <t>0:30:51</t>
         </is>
       </c>
       <c r="G38" t="b">
@@ -1988,19 +1988,19 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=too</t>
+          <t>https://www.nationstates.net/region=tropical_islands</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>UnderBerg</t>
+          <t>The Federation of the FA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2009,27 +2009,27 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1735</v>
+        <v>1359</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0:28:55</t>
+          <t>0:22:39</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2602</v>
+        <v>2039</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0:43:22</t>
+          <t>0:33:59</t>
         </is>
       </c>
       <c r="G39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=underberg</t>
+          <t>https://www.nationstates.net/region=the_federation_of_the_fa</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2041,7 +2041,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>TSGAIN of Rayzonia</t>
+          <t>The Westerlands</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2050,27 +2050,27 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1767</v>
+        <v>1425</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0:29:27</t>
+          <t>0:23:45</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2650</v>
+        <v>2137</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0:44:10</t>
+          <t>0:35:37</t>
         </is>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=tsgain_of_rayzonia</t>
+          <t>https://www.nationstates.net/region=the_westerlands</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2082,28 +2082,28 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>my side of the world</t>
+          <t>The Region of Peace</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1769</v>
+        <v>1502</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0:29:29</t>
+          <t>0:25:02</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2653</v>
+        <v>2253</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0:44:13</t>
+          <t>0:37:33</t>
         </is>
       </c>
       <c r="G41" t="b">
@@ -2111,81 +2111,81 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=my_side_of_the_world</t>
+          <t>https://www.nationstates.net/region=the_region_of_peace</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>EPSA</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>SEVENUP</t>
+          <t>Interstate 878</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1800</v>
+        <v>1631</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0:30:00</t>
+          <t>0:27:11</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2700</v>
+        <v>2446</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0:45:00</t>
+          <t>0:40:46</t>
         </is>
       </c>
       <c r="G42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=sevenup</t>
+          <t>https://www.nationstates.net/region=interstate_878</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>BFL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Gulagia</t>
+          <t>Too</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1829</v>
+        <v>1631</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0:30:29</t>
+          <t>0:27:11</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2744</v>
+        <v>2447</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0:45:44</t>
+          <t>0:40:47</t>
         </is>
       </c>
       <c r="G43" t="b">
@@ -2193,19 +2193,19 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=gulagia</t>
+          <t>https://www.nationstates.net/region=too</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>United Governments of NationStates</t>
+          <t>UnderBerg</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2214,101 +2214,101 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1848</v>
+        <v>1735</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0:30:48</t>
+          <t>0:28:55</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2772</v>
+        <v>2602</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0:46:12</t>
+          <t>0:43:22</t>
         </is>
       </c>
       <c r="G44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=united_governments_of_nationstates</t>
+          <t>https://www.nationstates.net/region=underberg</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Union of Confederate Regions</t>
+          <t>TSGAIN of Rayzonia</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1851</v>
+        <v>1767</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0:30:51</t>
+          <t>0:29:27</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2777</v>
+        <v>2650</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0:46:17</t>
+          <t>0:44:10</t>
         </is>
       </c>
       <c r="G45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_confederate_regions</t>
+          <t>https://www.nationstates.net/region=tsgain_of_rayzonia</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>SolarFlare</t>
+          <t>my side of the world</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1867</v>
+        <v>1769</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0:31:07</t>
+          <t>0:29:29</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2800</v>
+        <v>2653</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0:46:40</t>
+          <t>0:44:13</t>
         </is>
       </c>
       <c r="G46" t="b">
@@ -2316,40 +2316,40 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=solarflare</t>
+          <t>https://www.nationstates.net/region=my_side_of_the_world</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>EPSA</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>The Mass Effect Universe</t>
+          <t>Obama Islands</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1872</v>
+        <v>1779</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0:31:12</t>
+          <t>0:29:39</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2808</v>
+        <v>2668</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0:46:48</t>
+          <t>0:44:28</t>
         </is>
       </c>
       <c r="G47" t="b">
@@ -2357,81 +2357,81 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_mass_effect_universe</t>
+          <t>https://www.nationstates.net/region=obama_islands</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>BFL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Regional Officers</t>
+          <t>SEVENUP</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1882</v>
+        <v>1800</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0:31:22</t>
+          <t>0:30:00</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2824</v>
+        <v>2700</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0:47:04</t>
+          <t>0:45:00</t>
         </is>
       </c>
       <c r="G48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=regional_officers</t>
+          <t>https://www.nationstates.net/region=sevenup</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Fallout DnD</t>
+          <t>Gulagia</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1892</v>
+        <v>1829</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0:31:32</t>
+          <t>0:30:29</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2838</v>
+        <v>2744</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0:47:18</t>
+          <t>0:45:44</t>
         </is>
       </c>
       <c r="G49" t="b">
@@ -2439,19 +2439,19 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=fallout_dnd</t>
+          <t>https://www.nationstates.net/region=gulagia</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Chippewa</t>
+          <t>United Governments of NationStates</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2460,19 +2460,19 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1903</v>
+        <v>1848</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0:31:43</t>
+          <t>0:30:48</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2855</v>
+        <v>2772</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0:47:35</t>
+          <t>0:46:12</t>
         </is>
       </c>
       <c r="G50" t="b">
@@ -2480,40 +2480,40 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=chippewa</t>
+          <t>https://www.nationstates.net/region=united_governments_of_nationstates</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Korel</t>
+          <t>Union of Confederate Regions</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1921</v>
+        <v>1851</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0:32:01</t>
+          <t>0:30:51</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2882</v>
+        <v>2777</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0:48:02</t>
+          <t>0:46:17</t>
         </is>
       </c>
       <c r="G51" t="b">
@@ -2521,40 +2521,40 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=korel</t>
+          <t>https://www.nationstates.net/region=union_of_confederate_regions</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>The Fortnite Multiverse</t>
+          <t>SolarFlare</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO, Embassies</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1947</v>
+        <v>1867</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0:32:27</t>
+          <t>0:31:07</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2920</v>
+        <v>2800</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0:48:40</t>
+          <t>0:46:40</t>
         </is>
       </c>
       <c r="G52" t="b">
@@ -2562,19 +2562,19 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_fortnite_multiverse</t>
+          <t>https://www.nationstates.net/region=solarflare</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>KstewF04</t>
+          <t>The Mass Effect Universe</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2583,19 +2583,19 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1964</v>
+        <v>1872</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0:32:44</t>
+          <t>0:31:12</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>2947</v>
+        <v>2808</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0:49:07</t>
+          <t>0:46:48</t>
         </is>
       </c>
       <c r="G53" t="b">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kstewf04</t>
+          <t>https://www.nationstates.net/region=the_mass_effect_universe</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2615,28 +2615,28 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>The Confederation Of Nations</t>
+          <t>Regional Officers</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1982</v>
+        <v>1882</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0:33:02</t>
+          <t>0:31:22</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>2973</v>
+        <v>2824</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0:49:33</t>
+          <t>0:47:04</t>
         </is>
       </c>
       <c r="G54" t="b">
@@ -2644,60 +2644,60 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_confederation_of_nations</t>
+          <t>https://www.nationstates.net/region=regional_officers</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Big Man Anarchy Union</t>
+          <t>Fallout DnD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2000</v>
+        <v>1892</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0:33:20</t>
+          <t>0:31:32</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>3001</v>
+        <v>2838</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0:50:01</t>
+          <t>0:47:18</t>
         </is>
       </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=big_man_anarchy_union</t>
+          <t>https://www.nationstates.net/region=fallout_dnd</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>BoM, TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Soodan</t>
+          <t>Chippewa</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2706,27 +2706,27 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2179</v>
+        <v>1903</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0:36:19</t>
+          <t>0:31:43</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>3268</v>
+        <v>2855</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0:54:28</t>
+          <t>0:47:35</t>
         </is>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=soodan</t>
+          <t>https://www.nationstates.net/region=chippewa</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2738,28 +2738,28 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Malice Girl Scouts</t>
+          <t>Korel</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2180</v>
+        <v>1921</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0:36:20</t>
+          <t>0:32:01</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>3269</v>
+        <v>2882</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0:54:29</t>
+          <t>0:48:02</t>
         </is>
       </c>
       <c r="G57" t="b">
@@ -2767,19 +2767,19 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
+          <t>https://www.nationstates.net/region=korel</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Korovia</t>
+          <t>The Fortnite Multiverse</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2788,27 +2788,27 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2199</v>
+        <v>1947</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0:36:39</t>
+          <t>0:32:27</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>3299</v>
+        <v>2920</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0:54:59</t>
+          <t>0:48:40</t>
         </is>
       </c>
       <c r="G58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=korovia</t>
+          <t>https://www.nationstates.net/region=the_fortnite_multiverse</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2820,28 +2820,28 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Cretanja Queendom</t>
+          <t>KstewF04</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2216</v>
+        <v>1964</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0:36:56</t>
+          <t>0:32:44</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>3324</v>
+        <v>2947</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0:55:24</t>
+          <t>0:49:07</t>
         </is>
       </c>
       <c r="G59" t="b">
@@ -2849,19 +2849,19 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cretanja_queendom</t>
+          <t>https://www.nationstates.net/region=kstewf04</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Iron Front</t>
+          <t>The Confederation Of Nations</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2870,27 +2870,27 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2216</v>
+        <v>1982</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0:36:56</t>
+          <t>0:33:02</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>3324</v>
+        <v>2973</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0:55:24</t>
+          <t>0:49:33</t>
         </is>
       </c>
       <c r="G60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=iron_front</t>
+          <t>https://www.nationstates.net/region=the_confederation_of_nations</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2902,110 +2902,110 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>The Collective</t>
+          <t>Big Man Anarchy Union</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2221</v>
+        <v>2000</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0:37:01</t>
+          <t>0:33:20</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>3331</v>
+        <v>3001</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0:55:31</t>
+          <t>0:50:01</t>
         </is>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_collective</t>
+          <t>https://www.nationstates.net/region=big_man_anarchy_union</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Malphe</t>
+          <t>Soodan</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2559</v>
+        <v>2179</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0:42:39</t>
+          <t>0:36:19</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>3838</v>
+        <v>3268</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1:03:58</t>
+          <t>0:54:28</t>
         </is>
       </c>
       <c r="G62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=malphe</t>
+          <t>https://www.nationstates.net/region=soodan</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Lily, Osiris</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Submissive and Raidable</t>
+          <t>The Brotherhood of Malice Girl Scouts</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2771</v>
+        <v>2180</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0:46:11</t>
+          <t>0:36:20</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>4157</v>
+        <v>3269</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>1:09:17</t>
+          <t>0:54:29</t>
         </is>
       </c>
       <c r="G63" t="b">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3025,80 +3025,367 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Eastern American Union</t>
+          <t>Korovia</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2816</v>
+        <v>2199</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0:46:56</t>
+          <t>0:36:39</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>4223</v>
+        <v>3299</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>1:10:23</t>
+          <t>0:54:59</t>
         </is>
       </c>
       <c r="G64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=eastern_american_union</t>
+          <t>https://www.nationstates.net/region=korovia</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>BoM, TBH</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
+          <t>Cretanja Queendom</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>2216</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0:36:56</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>3324</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>0:55:24</t>
+        </is>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=cretanja_queendom</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Iron Front</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>WFE, Embassies</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>2216</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0:36:56</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>3324</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0:55:24</t>
+        </is>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=iron_front</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>BoM, TBH</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>The Collective</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>2221</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0:37:01</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>3331</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>0:55:31</t>
+        </is>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=the_collective</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Lily</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Malphe</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>2559</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0:42:39</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>3838</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>1:03:58</t>
+        </is>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=malphe</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Lily, Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Submissive and Raidable</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>2771</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0:46:11</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>4157</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>1:09:17</t>
+        </is>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>BoM</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>Eastern American Union</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>2816</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0:46:56</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>4223</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1:10:23</t>
+        </is>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=eastern_american_union</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Lily, TBH</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>The Boy Band</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3062</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0:51:02</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>4594</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>1:16:34</t>
+        </is>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=the_boy_band</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>NPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
           <t>Brest Oblast</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B72" t="inlineStr">
         <is>
           <t>Embassies</t>
         </is>
       </c>
-      <c r="C65" t="n">
+      <c r="C72" t="n">
         <v>3449</v>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>0:57:29</t>
         </is>
       </c>
-      <c r="E65" t="n">
+      <c r="E72" t="n">
         <v>5174</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>1:26:14</t>
         </is>
       </c>
-      <c r="G65" t="b">
-        <v>0</v>
-      </c>
-      <c r="H65" t="inlineStr">
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="inlineStr">
         <is>
           <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="I72" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Flag more RO names
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,28 +606,28 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>The Koprulu Sector</t>
+          <t>abolished</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>WFE, Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0:02:52</t>
+          <t>0:02:17</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>258</v>
+        <v>206</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:04:18</t>
+          <t>0:03:26</t>
         </is>
       </c>
       <c r="G5" t="b">
@@ -635,40 +635,40 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
+          <t>https://www.nationstates.net/region=abolished</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>United Fascist Territory of Waschuster</t>
+          <t>The Koprulu Sector</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>WFE, Embassies</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>237</v>
+        <v>172</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0:03:57</t>
+          <t>0:02:52</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>355</v>
+        <v>258</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:05:55</t>
+          <t>0:04:18</t>
         </is>
       </c>
       <c r="G6" t="b">
@@ -676,40 +676,40 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=united_fascist_territory_of_waschuster</t>
+          <t>https://www.nationstates.net/region=the_koprulu_sector</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>region with the word Tractor in it</t>
+          <t>United Fascist Territory of Waschuster</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0:04:11</t>
+          <t>0:03:57</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:06:16</t>
+          <t>0:05:55</t>
         </is>
       </c>
       <c r="G7" t="b">
@@ -717,40 +717,40 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
+          <t>https://www.nationstates.net/region=united_fascist_territory_of_waschuster</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>The west germanic provinces</t>
+          <t>region with the word Tractor in it</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>306</v>
+        <v>251</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0:05:06</t>
+          <t>0:04:11</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>460</v>
+        <v>376</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:07:40</t>
+          <t>0:06:16</t>
         </is>
       </c>
       <c r="G8" t="b">
@@ -758,40 +758,40 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
+          <t>https://www.nationstates.net/region=region_with_the_word_tractor_in_it</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Commonwealth of Diverse Nations</t>
+          <t>The west germanic provinces</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>351</v>
+        <v>306</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0:05:51</t>
+          <t>0:05:06</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>526</v>
+        <v>460</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:08:46</t>
+          <t>0:07:40</t>
         </is>
       </c>
       <c r="G9" t="b">
@@ -799,40 +799,40 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
+          <t>https://www.nationstates.net/region=the_west_germanic_provinces</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>BoM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>The Great States of Fascist Nudists</t>
+          <t>Commonwealth of Diverse Nations</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>WFE, RO, Embassies</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>470</v>
+        <v>351</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0:07:50</t>
+          <t>0:05:51</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>704</v>
+        <v>526</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:11:44</t>
+          <t>0:08:46</t>
         </is>
       </c>
       <c r="G10" t="b">
@@ -840,40 +840,40 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
+          <t>https://www.nationstates.net/region=commonwealth_of_diverse_nations</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Aerope</t>
+          <t>Zolochiv</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1234</v>
+        <v>421</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0:20:34</t>
+          <t>0:07:01</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1851</v>
+        <v>631</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:30:51</t>
+          <t>0:10:31</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -881,40 +881,40 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=aerope</t>
+          <t>https://www.nationstates.net/region=zolochiv</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Kyorgia puppet storage</t>
+          <t>The Great States of Fascist Nudists</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>WFE, RO, Embassies</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1239</v>
+        <v>470</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0:20:39</t>
+          <t>0:07:50</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1859</v>
+        <v>704</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:30:59</t>
+          <t>0:11:44</t>
         </is>
       </c>
       <c r="G12" t="b">
@@ -922,19 +922,19 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
+          <t>https://www.nationstates.net/region=the_great_states_of_fascist_nudists</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>EPSA, Lily, Osiris, TBH</t>
+          <t>BoM, Lily, Osiris, Sparkalia, TBH</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Blood</t>
+          <t>Propounded Empathy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1248</v>
+        <v>733</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0:20:48</t>
+          <t>0:12:13</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1872</v>
+        <v>1099</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:31:12</t>
+          <t>0:18:19</t>
         </is>
       </c>
       <c r="G13" t="b">
@@ -963,7 +963,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
+          <t>https://www.nationstates.net/region=propounded_empathy</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -975,7 +975,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>abrogated</t>
+          <t>Crazed Nations CN</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -984,19 +984,19 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1741</v>
+        <v>1087</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0:29:01</t>
+          <t>0:18:07</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2611</v>
+        <v>1631</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:43:31</t>
+          <t>0:27:11</t>
         </is>
       </c>
       <c r="G14" t="b">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=abrogated</t>
+          <t>https://www.nationstates.net/region=crazed_nations_cn</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1016,7 +1016,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Union of Confederate Regions</t>
+          <t>Aerope</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1025,19 +1025,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1841</v>
+        <v>1234</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0:30:41</t>
+          <t>0:20:34</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2762</v>
+        <v>1851</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:46:02</t>
+          <t>0:30:51</t>
         </is>
       </c>
       <c r="G15" t="b">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=union_of_confederate_regions</t>
+          <t>https://www.nationstates.net/region=aerope</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1057,48 +1057,48 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Erynia Card Farm</t>
+          <t>Kyorgia puppet storage</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WFE, RO</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1882</v>
+        <v>1239</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0:31:22</t>
+          <t>0:20:39</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2824</v>
+        <v>1859</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:47:04</t>
+          <t>0:30:59</t>
         </is>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=erynia_card_farm</t>
+          <t>https://www.nationstates.net/region=kyorgia_puppet_storage</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TBH</t>
+          <t>EPSA, Lily, Osiris, TBH</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>The Sercia canal</t>
+          <t>The Brotherhood of Blood</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1107,19 +1107,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1934</v>
+        <v>1248</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0:32:14</t>
+          <t>0:20:48</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2901</v>
+        <v>1872</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:48:21</t>
+          <t>0:31:12</t>
         </is>
       </c>
       <c r="G17" t="b">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_sercia_canal</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_blood</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1139,28 +1139,28 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>The Brotherhood of Malice Girl Scouts</t>
+          <t>abrogated</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2255</v>
+        <v>1741</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0:37:35</t>
+          <t>0:29:01</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3382</v>
+        <v>2611</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0:56:22</t>
+          <t>0:43:31</t>
         </is>
       </c>
       <c r="G18" t="b">
@@ -1168,19 +1168,19 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
+          <t>https://www.nationstates.net/region=abrogated</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>BoM</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Cretanja Queendom</t>
+          <t>Union of Confederate Regions</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1189,101 +1189,101 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2296</v>
+        <v>1841</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0:38:16</t>
+          <t>0:30:41</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3443</v>
+        <v>2762</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0:57:23</t>
+          <t>0:46:02</t>
         </is>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=cretanja_queendom</t>
+          <t>https://www.nationstates.net/region=union_of_confederate_regions</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>Sparkalia</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>The Collective</t>
+          <t>Erynia Card Farm</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>WFE, RO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2301</v>
+        <v>1882</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0:38:21</t>
+          <t>0:31:22</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>3451</v>
+        <v>2824</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0:57:31</t>
+          <t>0:47:04</t>
         </is>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=the_collective</t>
+          <t>https://www.nationstates.net/region=erynia_card_farm</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>TBH</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Malphe</t>
+          <t>The Sercia canal</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Embassies</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2699</v>
+        <v>1934</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0:44:59</t>
+          <t>0:32:14</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>4049</v>
+        <v>2901</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1:07:29</t>
+          <t>0:48:21</t>
         </is>
       </c>
       <c r="G21" t="b">
@@ -1291,40 +1291,40 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=malphe</t>
+          <t>https://www.nationstates.net/region=the_sercia_canal</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Lily, Osiris</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Submissive and Raidable</t>
+          <t>The Brotherhood of Malice Girl Scouts</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2908</v>
+        <v>2255</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0:48:28</t>
+          <t>0:37:35</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>4363</v>
+        <v>3382</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1:12:43</t>
+          <t>0:56:22</t>
         </is>
       </c>
       <c r="G22" t="b">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+          <t>https://www.nationstates.net/region=the_brotherhood_of_malice_girl_scouts</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1344,80 +1344,244 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Eastern American Union</t>
+          <t>Cretanja Queendom</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>WFE</t>
+          <t>Embassies</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2956</v>
+        <v>2296</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0:49:16</t>
+          <t>0:38:16</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4434</v>
+        <v>3443</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1:13:54</t>
+          <t>0:57:23</t>
         </is>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.nationstates.net/region=eastern_american_union</t>
+          <t>https://www.nationstates.net/region=cretanja_queendom</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Lily, TBH</t>
+          <t>Osiris</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
+          <t>The Collective</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2301</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0:38:21</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>3451</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0:57:31</t>
+        </is>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=the_collective</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Lily</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Malphe</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Embassies</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2699</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0:44:59</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>4049</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1:07:29</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=malphe</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Lily, Osiris</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Submissive and Raidable</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2908</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0:48:28</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>4363</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1:12:43</t>
+        </is>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=submissive_and_raidable</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>BoM</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Eastern American Union</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>WFE</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2956</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0:49:16</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>4434</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>1:13:54</t>
+        </is>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://www.nationstates.net/region=eastern_american_union</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Lily, TBH</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
           <t>Brest Oblast</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Embassies</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C28" t="n">
         <v>3456</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>0:57:36</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="E28" t="n">
         <v>5184</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>1:26:24</t>
         </is>
       </c>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" t="inlineStr">
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>https://www.nationstates.net/region=brest_oblast</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>EPSA, Lily</t>
         </is>

</xml_diff>

<commit_message>
Update TCB embassy flagging
</commit_message>
<xml_diff>
--- a/data/detags.xlsx
+++ b/data/detags.xlsx
@@ -681,7 +681,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Osiris</t>
+          <t>Osiris, TCB</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Osiris, TBH</t>
+          <t>Osiris, TBH, TCB</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Sparkalia</t>
+          <t>Sparkalia, TCB</t>
         </is>
       </c>
     </row>

</xml_diff>